<commit_message>
added fpga unoptimised in excel
</commit_message>
<xml_diff>
--- a/lab3/lsal/lab3 LSAL imlementation.xlsx
+++ b/lab3/lsal/lab3 LSAL imlementation.xlsx
@@ -1,17 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <workbookPr defaultThemeVersion="202300"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sstat\Documents\GitHub\Embedded-Systems\lab3\lsal\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365CE0C9-DB29-474C-B90A-C46232C43CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Φύλλο1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Φύλλο1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -20,45 +36,50 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="11">
   <si>
-    <t xml:space="preserve">x86</t>
+    <t>x86</t>
   </si>
   <si>
-    <t xml:space="preserve">ARM</t>
+    <t>ARM</t>
   </si>
   <si>
-    <t xml:space="preserve">Ν</t>
+    <t>Ν</t>
   </si>
   <si>
-    <t xml:space="preserve">Μ</t>
+    <t>Μ</t>
   </si>
   <si>
-    <t xml:space="preserve">unoptimised (s)</t>
+    <t>unoptimised (s)</t>
   </si>
   <si>
-    <t xml:space="preserve">optimised (s)</t>
+    <t>optimised (s)</t>
   </si>
   <si>
-    <t xml:space="preserve">Optimisation</t>
+    <t>Optimisation</t>
   </si>
   <si>
-    <t xml:space="preserve">x86 vs ARM Optimised</t>
+    <t>x86 vs ARM Optimised</t>
   </si>
   <si>
-    <t xml:space="preserve">x86 vs ARM Unoptimised</t>
+    <t>x86 vs ARM Unoptimised</t>
+  </si>
+  <si>
+    <t>FPGA</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.0000%"/>
-    <numFmt numFmtId="166" formatCode="#,##0.000000"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0000%"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000000"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -67,22 +88,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="22"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
@@ -90,34 +96,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="20"/>
-      <color rgb="FF595959"/>
-      <name val="Aptos Display"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF595959"/>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF595959"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF595959"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF595959"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -135,97 +117,55 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF232627"/>
-          <bgColor rgb="FFFCFCFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -284,15 +224,33 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -301,7 +259,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" lang="en-US" sz="2000" spc="-1" strike="noStrike">
+              <a:defRPr lang="en-US" sz="2000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -309,7 +267,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" lang="en-US" sz="2000" spc="-1" strike="noStrike">
+              <a:rPr lang="en-US" sz="2000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -330,6 +288,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -348,12 +307,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="196b24"/>
-            </a:solidFill>
-            <a:ln cap="rnd" w="38160">
+            <a:ln w="38160" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="196b24"/>
+                <a:srgbClr val="196B24"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -362,18 +318,26 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -382,8 +346,9 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
-            <c:showLeaderLines val="1"/>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
@@ -433,21 +398,26 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.3E-005</c:v>
+                  <c:v>1.2999999999999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.034103</c:v>
+                  <c:v>3.4103000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.263528</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.196854</c:v>
+                  <c:v>0.26352799999999998</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="#,##0.000000">
+                  <c:v>1.1968540000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C7F8-4A8A-A239-4F4C9BBD65C2}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -464,12 +434,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="0f9ed5"/>
-            </a:solidFill>
-            <a:ln cap="rnd" w="38160">
+            <a:ln w="38160" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="0f9ed5"/>
+                <a:srgbClr val="0F9ED5"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -478,18 +445,26 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -498,8 +473,9 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
-            <c:showLeaderLines val="1"/>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
@@ -549,22 +525,35 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.2E-005</c:v>
+                  <c:v>1.2E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.018605</c:v>
+                  <c:v>1.8605E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.137813</c:v>
+                  <c:v>0.13781299999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.628575</c:v>
+                  <c:v>0.62857499999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C7F8-4A8A-A239-4F4C9BBD65C2}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
             <a:ln w="0">
@@ -572,7 +561,7 @@
             </a:ln>
           </c:spPr>
         </c:hiLowLines>
-        <c:marker val="0"/>
+        <c:smooth val="0"/>
         <c:axId val="37655487"/>
         <c:axId val="33766647"/>
       </c:lineChart>
@@ -590,7 +579,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -598,7 +587,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -624,7 +613,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
+              <a:srgbClr val="D9D9D9"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -634,13 +623,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Aptos Narrow"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="33766647"/>
@@ -661,7 +651,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -671,7 +661,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="f2f2f2"/>
+                <a:srgbClr val="F2F2F2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -684,7 +674,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -692,7 +682,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -725,13 +715,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Aptos Narrow"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="37655487"/>
@@ -759,37 +750,46 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+            <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
               <a:solidFill>
                 <a:srgbClr val="595959"/>
               </a:solidFill>
               <a:latin typeface="Aptos Narrow"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln w="9360">
       <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
+        <a:srgbClr val="D9D9D9"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -798,7 +798,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" lang="en-US" sz="1400" spc="-1" strike="noStrike">
+              <a:defRPr lang="en-US" sz="1400" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -806,7 +806,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" lang="en-US" sz="1400" spc="-1" strike="noStrike">
+              <a:rPr lang="en-US" sz="1400" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -827,6 +827,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -845,12 +846,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="196b24"/>
-            </a:solidFill>
-            <a:ln cap="rnd" w="28440">
+            <a:ln w="28440" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="196b24"/>
+                <a:srgbClr val="196B24"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -859,18 +857,26 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -879,8 +885,9 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
-            <c:showLeaderLines val="1"/>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
@@ -930,21 +937,26 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4.5E-005</c:v>
+                  <c:v>4.5000000000000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.076079</c:v>
+                  <c:v>7.6078999999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.586488</c:v>
+                  <c:v>0.58648800000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.685104</c:v>
+                  <c:v>2.6851039999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AB4C-4C22-950D-04C7BD86A8F5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -961,12 +973,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="0f9ed5"/>
-            </a:solidFill>
-            <a:ln cap="rnd" w="28440">
+            <a:ln w="28440" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="0f9ed5"/>
+                <a:srgbClr val="0F9ED5"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -975,18 +984,26 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -995,8 +1012,9 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
-            <c:showLeaderLines val="1"/>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
@@ -1046,22 +1064,35 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.2E-005</c:v>
+                  <c:v>1.2E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.018605</c:v>
+                  <c:v>1.8605E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.137813</c:v>
+                  <c:v>0.13781299999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.628575</c:v>
+                  <c:v>0.62857499999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AB4C-4C22-950D-04C7BD86A8F5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
             <a:ln w="0">
@@ -1069,7 +1100,7 @@
             </a:ln>
           </c:spPr>
         </c:hiLowLines>
-        <c:marker val="0"/>
+        <c:smooth val="0"/>
         <c:axId val="92450187"/>
         <c:axId val="16042312"/>
       </c:lineChart>
@@ -1087,7 +1118,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="800" spc="-1" strike="noStrike">
+                  <a:defRPr lang="en-US" sz="800" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1095,7 +1126,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" lang="en-US" sz="800" spc="-1" strike="noStrike">
+                  <a:rPr lang="en-US" sz="800" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1121,7 +1152,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
+              <a:srgbClr val="D9D9D9"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1131,13 +1162,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Aptos Narrow"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="16042312"/>
@@ -1158,7 +1190,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1171,7 +1203,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr lang="en-US" sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1179,7 +1211,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
+                  <a:rPr lang="en-US" sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1212,13 +1244,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Aptos Narrow"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="92450187"/>
@@ -1246,37 +1279,46 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+            <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
               <a:solidFill>
                 <a:srgbClr val="595959"/>
               </a:solidFill>
               <a:latin typeface="Aptos Narrow"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln w="9360">
       <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
+        <a:srgbClr val="D9D9D9"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1285,7 +1327,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" lang="en-US" sz="2000" spc="-1" strike="noStrike">
+              <a:defRPr lang="en-US" sz="2000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1293,7 +1335,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" lang="en-US" sz="2000" spc="-1" strike="noStrike">
+              <a:rPr lang="en-US" sz="2000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1314,6 +1356,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -1332,10 +1375,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="156082"/>
-            </a:solidFill>
-            <a:ln cap="rnd" w="38160">
+            <a:ln w="38160" cap="rnd">
               <a:solidFill>
                 <a:srgbClr val="156082"/>
               </a:solidFill>
@@ -1346,18 +1386,26 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -1366,8 +1414,9 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
-            <c:showLeaderLines val="1"/>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
@@ -1417,21 +1466,26 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>9.8E-005</c:v>
+                  <c:v>9.7999999999999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.175177</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.402216</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.417753</c:v>
+                  <c:v>1.4022159999999999</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="#,##0.000000">
+                  <c:v>6.4177530000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-34CB-4835-8815-8C916767A52E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1448,12 +1502,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="196b24"/>
-            </a:solidFill>
-            <a:ln cap="rnd" w="38160">
+            <a:ln w="38160" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="196b24"/>
+                <a:srgbClr val="196B24"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1462,18 +1513,26 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -1482,8 +1541,9 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
-            <c:showLeaderLines val="1"/>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
@@ -1533,22 +1593,35 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.3E-005</c:v>
+                  <c:v>1.2999999999999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.034103</c:v>
+                  <c:v>3.4103000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.263528</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.196854</c:v>
+                  <c:v>0.26352799999999998</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="#,##0.000000">
+                  <c:v>1.1968540000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-34CB-4835-8815-8C916767A52E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
             <a:ln w="0">
@@ -1556,7 +1629,7 @@
             </a:ln>
           </c:spPr>
         </c:hiLowLines>
-        <c:marker val="0"/>
+        <c:smooth val="0"/>
         <c:axId val="54063989"/>
         <c:axId val="36264522"/>
       </c:lineChart>
@@ -1574,7 +1647,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1582,7 +1655,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1608,7 +1681,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
+              <a:srgbClr val="D9D9D9"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1618,13 +1691,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Aptos Narrow"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="36264522"/>
@@ -1645,7 +1719,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1655,7 +1729,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="f2f2f2"/>
+                <a:srgbClr val="F2F2F2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1668,7 +1742,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1676,7 +1750,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1709,13 +1783,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Aptos Narrow"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="54063989"/>
@@ -1743,37 +1818,46 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+            <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
               <a:solidFill>
                 <a:srgbClr val="595959"/>
               </a:solidFill>
               <a:latin typeface="Aptos Narrow"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln w="9360">
       <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
+        <a:srgbClr val="D9D9D9"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1782,7 +1866,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" lang="en-US" sz="2000" spc="-1" strike="noStrike">
+              <a:defRPr lang="en-US" sz="2000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1790,7 +1874,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" lang="en-US" sz="2000" spc="-1" strike="noStrike">
+              <a:rPr lang="en-US" sz="2000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1805,8 +1889,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.430195381882771"/>
-          <c:y val="0.0281510544384502"/>
+          <c:x val="0.43019538188277101"/>
+          <c:y val="2.8151054438450202E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1819,6 +1903,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -1837,10 +1922,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="156082"/>
-            </a:solidFill>
-            <a:ln cap="rnd" w="38160">
+            <a:ln w="38160" cap="rnd">
               <a:solidFill>
                 <a:srgbClr val="156082"/>
               </a:solidFill>
@@ -1851,18 +1933,26 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -1871,8 +1961,9 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
-            <c:showLeaderLines val="1"/>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
@@ -1922,21 +2013,26 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>9.8E-005</c:v>
+                  <c:v>9.7999999999999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.175177</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.402216</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.417753</c:v>
+                  <c:v>1.4022159999999999</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="#,##0.000000">
+                  <c:v>6.4177530000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B8A2-44DF-A1A8-5BDE6C04A60D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1953,12 +2049,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="e97132"/>
-            </a:solidFill>
-            <a:ln cap="rnd" w="38160">
+            <a:ln w="38160" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="e97132"/>
+                <a:srgbClr val="E97132"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1967,18 +2060,26 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -1987,8 +2088,9 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
-            <c:showLeaderLines val="1"/>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
@@ -2038,22 +2140,35 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4.5E-005</c:v>
+                  <c:v>4.5000000000000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.076079</c:v>
+                  <c:v>7.6078999999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.586488</c:v>
+                  <c:v>0.58648800000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.685104</c:v>
+                  <c:v>2.6851039999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B8A2-44DF-A1A8-5BDE6C04A60D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
             <a:ln w="0">
@@ -2061,7 +2176,7 @@
             </a:ln>
           </c:spPr>
         </c:hiLowLines>
-        <c:marker val="0"/>
+        <c:smooth val="0"/>
         <c:axId val="10855597"/>
         <c:axId val="79791227"/>
       </c:lineChart>
@@ -2079,7 +2194,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -2087,7 +2202,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -2113,7 +2228,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
+              <a:srgbClr val="D9D9D9"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -2123,13 +2238,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Aptos Narrow"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="79791227"/>
@@ -2150,7 +2266,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2160,7 +2276,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="f2f2f2"/>
+                <a:srgbClr val="F2F2F2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2173,7 +2289,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -2181,7 +2297,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -2214,13 +2330,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Aptos Narrow"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="10855597"/>
@@ -2248,35 +2365,42 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+            <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
               <a:solidFill>
                 <a:srgbClr val="595959"/>
               </a:solidFill>
               <a:latin typeface="Aptos Narrow"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln w="9360">
       <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
+        <a:srgbClr val="D9D9D9"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -2290,14 +2414,20 @@
       <xdr:row>27</xdr:row>
       <xdr:rowOff>14760</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Γράφημα 1"/>
+        <xdr:cNvPr id="2" name="Γράφημα 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="38160" y="1274400"/>
-        <a:ext cx="9868320" cy="3807720"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2320,14 +2450,20 @@
       <xdr:row>57</xdr:row>
       <xdr:rowOff>113760</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name="Γράφημα 3"/>
+        <xdr:cNvPr id="3" name="Γράφημα 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="6940440"/>
-        <a:ext cx="9964800" cy="3850920"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2350,14 +2486,20 @@
       <xdr:row>58</xdr:row>
       <xdr:rowOff>24840</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 4"/>
+        <xdr:cNvPr id="4" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11932200" y="6778440"/>
-        <a:ext cx="11657880" cy="4105080"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2380,14 +2522,20 @@
       <xdr:row>26</xdr:row>
       <xdr:rowOff>139320</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 5"/>
+        <xdr:cNvPr id="5" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11913480" y="1355760"/>
-        <a:ext cx="11147040" cy="3669840"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2412,11 +2560,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Image 1" descr=""/>
+        <xdr:cNvPr id="6" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -2438,83 +2592,420 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:E6" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A2:E6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Πίνακας1" displayName="Πίνακας1" ref="A2:E6" totalsRowShown="0">
+  <autoFilter ref="A2:E6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Ν"/>
-    <tableColumn id="2" name="Μ"/>
-    <tableColumn id="3" name="unoptimised (s)"/>
-    <tableColumn id="4" name="optimised (s)"/>
-    <tableColumn id="5" name="Optimisation"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Ν"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Μ"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="unoptimised (s)"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="optimised (s)"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Optimisation"/>
   </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Πίνακας13" displayName="Πίνακας13" ref="I2:M6" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="I2:M6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Πίνακας13" displayName="Πίνακας13" ref="I2:M6" totalsRowShown="0">
+  <autoFilter ref="I2:M6" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Ν"/>
-    <tableColumn id="2" name="Μ"/>
-    <tableColumn id="3" name="unoptimised (s)"/>
-    <tableColumn id="4" name="optimised (s)"/>
-    <tableColumn id="5" name="Optimisation"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Ν"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Μ"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="unoptimised (s)"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="optimised (s)"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Optimisation"/>
   </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Πίνακας14" displayName="Πίνακας14" ref="A31:E35" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A31:E35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Πίνακας14" displayName="Πίνακας14" ref="A31:E35" totalsRowShown="0">
+  <autoFilter ref="A31:E35" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Ν"/>
-    <tableColumn id="2" name="Μ"/>
-    <tableColumn id="3" name="ARM"/>
-    <tableColumn id="4" name="x86"/>
-    <tableColumn id="5" name="Optimisation"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Ν"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Μ"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="ARM"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="x86"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Optimisation"/>
   </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Πίνακας145" displayName="Πίνακας145" ref="I31:M35" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="I31:M35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Πίνακας145" displayName="Πίνακας145" ref="I31:M35" totalsRowShown="0">
+  <autoFilter ref="I31:M35" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Ν"/>
-    <tableColumn id="2" name="Μ"/>
-    <tableColumn id="3" name="ARM"/>
-    <tableColumn id="4" name="x86"/>
-    <tableColumn id="5" name="Optimisation"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Ν"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Μ"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="ARM"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="x86"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Optimisation"/>
   </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{BBB9185F-D35F-416C-87BB-DA0E801C76EA}" name="Πίνακας16" displayName="Πίνακας16" ref="Q2:U7" totalsRowShown="0">
+  <autoFilter ref="Q2:U7" xr:uid="{BBB9185F-D35F-416C-87BB-DA0E801C76EA}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{B32C2711-E73F-48C0-8E10-3B3C4A2A4F2C}" name="Ν"/>
+    <tableColumn id="2" xr3:uid="{50BBA07D-FED9-4634-A8E8-C93F7635D63A}" name="Μ"/>
+    <tableColumn id="3" xr3:uid="{E68DE86C-467D-453A-9A13-6F92B789EED4}" name="unoptimised (s)"/>
+    <tableColumn id="4" xr3:uid="{3E13CB95-663F-4974-BAF1-C7264EC34CEE}" name="optimised (s)"/>
+    <tableColumn id="5" xr3:uid="{3979F865-D60E-4250-87D0-04BF2169D47A}" name="Optimisation">
+      <calculatedColumnFormula>T3/S3</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="0E2841"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E8E8E8"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="156082"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="E97132"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="196B24"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="0F9ED5"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="A02B93"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="4EA72E"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="467886"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="96607D"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:M35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q121" activeCellId="0" sqref="Q121"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="29.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="44.67"/>
+    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.21875" customWidth="1"/>
+    <col min="4" max="4" width="30.21875" customWidth="1"/>
+    <col min="5" max="5" width="28.88671875" customWidth="1"/>
+    <col min="9" max="9" width="26.77734375" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" customWidth="1"/>
+    <col min="11" max="11" width="29.21875" customWidth="1"/>
+    <col min="12" max="12" width="23" customWidth="1"/>
+    <col min="13" max="13" width="44.6640625" customWidth="1"/>
+    <col min="17" max="17" width="16.88671875" customWidth="1"/>
+    <col min="18" max="18" width="20.6640625" customWidth="1"/>
+    <col min="19" max="19" width="22.77734375" customWidth="1"/>
+    <col min="20" max="20" width="27.44140625" customWidth="1"/>
+    <col min="21" max="21" width="26.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:21" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2529,8 +3020,15 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
+      <c r="Q1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2561,144 +3059,216 @@
       <c r="M2" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="Q2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>32</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="2">
         <v>32</v>
       </c>
-      <c r="C3" s="3" t="n">
-        <v>1.3E-005</v>
-      </c>
-      <c r="D3" s="3" t="n">
-        <v>1.2E-005</v>
-      </c>
-      <c r="E3" s="4" t="n">
-        <f aca="false">D3/C3</f>
-        <v>0.923076923076923</v>
-      </c>
-      <c r="I3" s="3" t="n">
+      <c r="C3" s="2">
+        <v>1.2999999999999999E-5</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.2E-5</v>
+      </c>
+      <c r="E3" s="3">
+        <f>D3/C3</f>
+        <v>0.92307692307692313</v>
+      </c>
+      <c r="I3" s="2">
         <v>32</v>
       </c>
-      <c r="J3" s="3" t="n">
+      <c r="J3" s="2">
         <v>32</v>
       </c>
-      <c r="K3" s="3" t="n">
-        <v>9.8E-005</v>
-      </c>
-      <c r="L3" s="3" t="n">
-        <v>4.5E-005</v>
-      </c>
-      <c r="M3" s="4" t="n">
-        <f aca="false">L3/K3</f>
-        <v>0.459183673469388</v>
+      <c r="K3" s="2">
+        <v>9.7999999999999997E-5</v>
+      </c>
+      <c r="L3" s="2">
+        <v>4.5000000000000003E-5</v>
+      </c>
+      <c r="M3" s="3">
+        <f>L3/K3</f>
+        <v>0.45918367346938782</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>32</v>
+      </c>
+      <c r="R3" s="2">
+        <v>32</v>
+      </c>
+      <c r="S3" s="2">
+        <v>2.5655640000000002E-3</v>
+      </c>
+      <c r="T3" s="2"/>
+      <c r="U3" s="3">
+        <f>T3/S3</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
         <v>32</v>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="2">
         <v>65536</v>
       </c>
-      <c r="C4" s="3" t="n">
-        <v>0.034103</v>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>0.018605</v>
-      </c>
-      <c r="E4" s="4" t="n">
-        <f aca="false">D4/C4</f>
-        <v>0.545553177139841</v>
-      </c>
-      <c r="I4" s="3" t="n">
+      <c r="C4" s="2">
+        <v>3.4103000000000001E-2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.8605E-2</v>
+      </c>
+      <c r="E4" s="3">
+        <f>D4/C4</f>
+        <v>0.54555317713984108</v>
+      </c>
+      <c r="I4" s="2">
         <v>32</v>
       </c>
-      <c r="J4" s="3" t="n">
+      <c r="J4" s="2">
         <v>65536</v>
       </c>
-      <c r="K4" s="3" t="n">
+      <c r="K4" s="2">
         <v>0.175177</v>
       </c>
-      <c r="L4" s="3" t="n">
-        <v>0.076079</v>
-      </c>
-      <c r="M4" s="4" t="n">
-        <f aca="false">L4/K4</f>
-        <v>0.434297881571211</v>
+      <c r="L4" s="2">
+        <v>7.6078999999999994E-2</v>
+      </c>
+      <c r="M4" s="3">
+        <f>L4/K4</f>
+        <v>0.4342978815712108</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>32</v>
+      </c>
+      <c r="R4" s="2">
+        <v>65536</v>
+      </c>
+      <c r="S4" s="2">
+        <v>2.6276989529999999</v>
+      </c>
+      <c r="T4" s="2"/>
+      <c r="U4" s="3">
+        <f>T4/S4</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>256</v>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="2">
         <v>65536</v>
       </c>
-      <c r="C5" s="3" t="n">
-        <v>0.263528</v>
-      </c>
-      <c r="D5" s="3" t="n">
-        <v>0.137813</v>
-      </c>
-      <c r="E5" s="4" t="n">
-        <f aca="false">D5/C5</f>
-        <v>0.522953917610273</v>
-      </c>
-      <c r="I5" s="3" t="n">
+      <c r="C5" s="2">
+        <v>0.26352799999999998</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.13781299999999999</v>
+      </c>
+      <c r="E5" s="3">
+        <f>D5/C5</f>
+        <v>0.52295391761027288</v>
+      </c>
+      <c r="I5" s="2">
         <v>256</v>
       </c>
-      <c r="J5" s="3" t="n">
+      <c r="J5" s="2">
         <v>65536</v>
       </c>
-      <c r="K5" s="3" t="n">
-        <v>1.402216</v>
-      </c>
-      <c r="L5" s="3" t="n">
-        <v>0.586488</v>
-      </c>
-      <c r="M5" s="4" t="n">
-        <f aca="false">L5/K5</f>
-        <v>0.418257957404565</v>
+      <c r="K5" s="2">
+        <v>1.4022159999999999</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0.58648800000000001</v>
+      </c>
+      <c r="M5" s="3">
+        <f>L5/K5</f>
+        <v>0.41825795740456539</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>256</v>
+      </c>
+      <c r="R5" s="2">
+        <v>65536</v>
+      </c>
+      <c r="S5" s="2">
+        <v>0.44895658399999999</v>
+      </c>
+      <c r="T5" s="2"/>
+      <c r="U5" s="3">
+        <f>T5/S5</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
         <v>256</v>
       </c>
-      <c r="B6" s="3" t="n">
+      <c r="B6" s="2">
         <v>300000</v>
       </c>
-      <c r="C6" s="5" t="n">
-        <v>1.196854</v>
-      </c>
-      <c r="D6" s="3" t="n">
-        <v>0.628575</v>
-      </c>
-      <c r="E6" s="4" t="n">
-        <f aca="false">D6/C6</f>
-        <v>0.525189371468867</v>
-      </c>
-      <c r="I6" s="3" t="n">
+      <c r="C6" s="4">
+        <v>1.1968540000000001</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.62857499999999999</v>
+      </c>
+      <c r="E6" s="3">
+        <f>D6/C6</f>
+        <v>0.52518937146886746</v>
+      </c>
+      <c r="I6" s="2">
         <v>256</v>
       </c>
-      <c r="J6" s="3" t="n">
+      <c r="J6" s="2">
         <v>300000</v>
       </c>
-      <c r="K6" s="5" t="n">
-        <v>6.417753</v>
-      </c>
-      <c r="L6" s="3" t="n">
-        <v>2.685104</v>
-      </c>
-      <c r="M6" s="4" t="n">
-        <f aca="false">L6/K6</f>
-        <v>0.418386933869222</v>
+      <c r="K6" s="4">
+        <v>6.4177530000000003</v>
+      </c>
+      <c r="L6" s="2">
+        <v>2.6851039999999999</v>
+      </c>
+      <c r="M6" s="3">
+        <f>L6/K6</f>
+        <v>0.41838693386922182</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>256</v>
+      </c>
+      <c r="R6" s="2">
+        <v>300000</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="U6" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
@@ -2714,7 +3284,7 @@
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
     </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>2</v>
       </c>
@@ -2746,162 +3316,160 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="n">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
         <v>32</v>
       </c>
-      <c r="B32" s="3" t="n">
+      <c r="B32" s="2">
         <v>32</v>
       </c>
-      <c r="C32" s="3" t="n">
-        <v>4.5E-005</v>
-      </c>
-      <c r="D32" s="3" t="n">
-        <v>1.2E-005</v>
-      </c>
-      <c r="E32" s="4" t="n">
-        <f aca="false">D32/C32</f>
-        <v>0.266666666666667</v>
-      </c>
-      <c r="I32" s="3" t="n">
+      <c r="C32" s="2">
+        <v>4.5000000000000003E-5</v>
+      </c>
+      <c r="D32" s="2">
+        <v>1.2E-5</v>
+      </c>
+      <c r="E32" s="3">
+        <f>D32/C32</f>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="I32" s="2">
         <v>32</v>
       </c>
-      <c r="J32" s="3" t="n">
+      <c r="J32" s="2">
         <v>32</v>
       </c>
-      <c r="K32" s="3" t="n">
-        <v>9.8E-005</v>
-      </c>
-      <c r="L32" s="3" t="n">
-        <v>1.3E-005</v>
-      </c>
-      <c r="M32" s="4" t="n">
-        <f aca="false">L32/K32</f>
-        <v>0.13265306122449</v>
+      <c r="K32" s="2">
+        <v>9.7999999999999997E-5</v>
+      </c>
+      <c r="L32" s="2">
+        <v>1.2999999999999999E-5</v>
+      </c>
+      <c r="M32" s="3">
+        <f>L32/K32</f>
+        <v>0.1326530612244898</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3" t="n">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
         <v>32</v>
       </c>
-      <c r="B33" s="3" t="n">
+      <c r="B33" s="2">
         <v>65536</v>
       </c>
-      <c r="C33" s="3" t="n">
-        <v>0.076079</v>
-      </c>
-      <c r="D33" s="3" t="n">
-        <v>0.018605</v>
-      </c>
-      <c r="E33" s="4" t="n">
-        <f aca="false">D33/C33</f>
-        <v>0.244548429921529</v>
-      </c>
-      <c r="I33" s="3" t="n">
+      <c r="C33" s="2">
+        <v>7.6078999999999994E-2</v>
+      </c>
+      <c r="D33" s="2">
+        <v>1.8605E-2</v>
+      </c>
+      <c r="E33" s="3">
+        <f>D33/C33</f>
+        <v>0.24454842992152895</v>
+      </c>
+      <c r="I33" s="2">
         <v>32</v>
       </c>
-      <c r="J33" s="3" t="n">
+      <c r="J33" s="2">
         <v>65536</v>
       </c>
-      <c r="K33" s="3" t="n">
+      <c r="K33" s="2">
         <v>0.175177</v>
       </c>
-      <c r="L33" s="3" t="n">
-        <v>0.034103</v>
-      </c>
-      <c r="M33" s="4" t="n">
-        <f aca="false">L33/K33</f>
-        <v>0.194677383446457</v>
+      <c r="L33" s="2">
+        <v>3.4103000000000001E-2</v>
+      </c>
+      <c r="M33" s="3">
+        <f>L33/K33</f>
+        <v>0.19467738344645702</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3" t="n">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
         <v>256</v>
       </c>
-      <c r="B34" s="3" t="n">
+      <c r="B34" s="2">
         <v>65536</v>
       </c>
-      <c r="C34" s="3" t="n">
-        <v>0.586488</v>
-      </c>
-      <c r="D34" s="3" t="n">
-        <v>0.137813</v>
-      </c>
-      <c r="E34" s="4" t="n">
-        <f aca="false">D34/C34</f>
-        <v>0.234980084844021</v>
-      </c>
-      <c r="I34" s="3" t="n">
+      <c r="C34" s="2">
+        <v>0.58648800000000001</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.13781299999999999</v>
+      </c>
+      <c r="E34" s="3">
+        <f>D34/C34</f>
+        <v>0.23498008484402066</v>
+      </c>
+      <c r="I34" s="2">
         <v>256</v>
       </c>
-      <c r="J34" s="3" t="n">
+      <c r="J34" s="2">
         <v>65536</v>
       </c>
-      <c r="K34" s="3" t="n">
-        <v>1.402216</v>
-      </c>
-      <c r="L34" s="3" t="n">
-        <v>0.263528</v>
-      </c>
-      <c r="M34" s="4" t="n">
-        <f aca="false">L34/K34</f>
-        <v>0.187936808594396</v>
+      <c r="K34" s="2">
+        <v>1.4022159999999999</v>
+      </c>
+      <c r="L34" s="2">
+        <v>0.26352799999999998</v>
+      </c>
+      <c r="M34" s="3">
+        <f>L34/K34</f>
+        <v>0.18793680859439629</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3" t="n">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
         <v>256</v>
       </c>
-      <c r="B35" s="3" t="n">
+      <c r="B35" s="2">
         <v>300000</v>
       </c>
-      <c r="C35" s="3" t="n">
-        <v>2.685104</v>
-      </c>
-      <c r="D35" s="3" t="n">
-        <v>0.628575</v>
-      </c>
-      <c r="E35" s="4" t="n">
-        <f aca="false">D35/C35</f>
-        <v>0.234097077804063</v>
-      </c>
-      <c r="I35" s="3" t="n">
+      <c r="C35" s="2">
+        <v>2.6851039999999999</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.62857499999999999</v>
+      </c>
+      <c r="E35" s="3">
+        <f>D35/C35</f>
+        <v>0.23409707780406272</v>
+      </c>
+      <c r="I35" s="2">
         <v>256</v>
       </c>
-      <c r="J35" s="3" t="n">
+      <c r="J35" s="2">
         <v>300000</v>
       </c>
-      <c r="K35" s="5" t="n">
-        <v>6.417753</v>
-      </c>
-      <c r="L35" s="5" t="n">
-        <v>1.196854</v>
-      </c>
-      <c r="M35" s="4" t="n">
-        <f aca="false">L35/K35</f>
-        <v>0.186491128592827</v>
+      <c r="K35" s="4">
+        <v>6.4177530000000003</v>
+      </c>
+      <c r="L35" s="4">
+        <v>1.1968540000000001</v>
+      </c>
+      <c r="M35" s="3">
+        <f>L35/K35</f>
+        <v>0.18649112859282682</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="I1:M1"/>
     <mergeCell ref="A30:E30"/>
     <mergeCell ref="I30:M30"/>
+    <mergeCell ref="Q1:U1"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <drawing r:id="rId1"/>
-  <tableParts>
+  <tableParts count="5">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fpga times added in excel
</commit_message>
<xml_diff>
--- a/lab3/lsal/lab3 LSAL imlementation.xlsx
+++ b/lab3/lsal/lab3 LSAL imlementation.xlsx
@@ -1,33 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Φύλλο1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Φύλλο1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="11">
   <si>
-    <t>x86</t>
+    <t xml:space="preserve">x86</t>
   </si>
   <si>
-    <t>ARM</t>
+    <t xml:space="preserve">ARM</t>
   </si>
   <si>
-    <t>FPGA</t>
+    <t xml:space="preserve">FPGA</t>
   </si>
   <si>
-    <t>Ν</t>
+    <t xml:space="preserve">Ν</t>
   </si>
   <si>
-    <t>Μ</t>
+    <t xml:space="preserve">Μ</t>
   </si>
   <si>
     <t xml:space="preserve">unoptimised (s)</t>
@@ -36,10 +43,10 @@
     <t xml:space="preserve">optimised (s)</t>
   </si>
   <si>
-    <t>Optimisation</t>
+    <t xml:space="preserve">Optimisation</t>
   </si>
   <si>
-    <t>-</t>
+    <t xml:space="preserve">-</t>
   </si>
   <si>
     <t xml:space="preserve">x86 vs ARM Optimized</t>
@@ -51,22 +58,72 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.0000%"/>
-    <numFmt numFmtId="165" formatCode="#,##0.000000"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.0000%"/>
+    <numFmt numFmtId="166" formatCode="#,##0.000000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="10">
     <font>
-      <sz val="11.000000"/>
-      <color indexed="64"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="22.000000"/>
-      <color indexed="64"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="22"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FF595959"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF595959"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF595959"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF595959"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF595959"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -79,81 +136,181 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="52"/>
+        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="2">
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal style="none"/>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+  <cellXfs count="9">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="164" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="165" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="165" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="164" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFF2F2F2"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF196B24"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF156082"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFD9D9D9"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF0F9ED5"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFC000"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFE97132"/>
+      <rgbColor rgb="FF595959"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -162,32 +319,29 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr lang="en-US" sz="2000" b="0" strike="noStrike" spc="-1">
+              <a:defRPr b="0" lang="en-US" sz="2000" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Aptos Display"/>
+                <a:ea typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="2000" b="0" strike="noStrike" spc="-1">
+              <a:rPr b="0" lang="en-US" sz="2000" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Aptos Display"/>
+                <a:ea typeface="Arial"/>
               </a:rPr>
               <a:t>LSAL performance on x86 </a:t>
             </a:r>
-            <a:endParaRPr/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
-      <c:spPr bwMode="auto">
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+      <c:spPr>
         <a:noFill/>
         <a:ln w="0">
           <a:noFill/>
@@ -196,7 +350,6 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -214,13 +367,13 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln w="38160" cap="rnd">
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="196b24"/>
+            </a:solidFill>
+            <a:ln cap="rnd" w="38160">
               <a:solidFill>
-                <a:srgbClr val="196B24"/>
+                <a:srgbClr val="196b24"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -229,40 +382,34 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
-            <c:dLblPos val="r"/>
-            <c:separator xml:space="preserve">; </c:separator>
-            <c:showBubbleSize val="1"/>
-            <c:showCatName val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:showLegendKey val="0"/>
-            <c:showPercent val="0"/>
-            <c:showSerName val="0"/>
-            <c:showVal val="0"/>
-            <c:spPr bwMode="auto">
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
@@ -307,7 +454,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.000013</c:v>
+                  <c:v>1.3E-005</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.034103</c:v>
@@ -315,7 +462,7 @@
                 <c:pt idx="2">
                   <c:v>0.263528</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="#,##0.000000">
+                <c:pt idx="3">
                   <c:v>1.196854</c:v>
                 </c:pt>
               </c:numCache>
@@ -337,13 +484,13 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln w="38160" cap="rnd">
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="0f9ed5"/>
+            </a:solidFill>
+            <a:ln cap="rnd" w="38160">
               <a:solidFill>
-                <a:srgbClr val="0F9ED5"/>
+                <a:srgbClr val="0f9ed5"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -352,40 +499,34 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
-            <c:dLblPos val="r"/>
-            <c:separator xml:space="preserve">; </c:separator>
-            <c:showBubbleSize val="1"/>
-            <c:showCatName val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:showLegendKey val="0"/>
-            <c:showPercent val="0"/>
-            <c:showSerName val="0"/>
-            <c:showVal val="0"/>
-            <c:spPr bwMode="auto">
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
@@ -430,7 +571,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.000012</c:v>
+                  <c:v>1.2E-005</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.018605</c:v>
@@ -446,31 +587,19 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showBubbleSize val="0"/>
-          <c:showCatName val="0"/>
-          <c:showLeaderLines val="0"/>
-          <c:showLegendKey val="0"/>
-          <c:showPercent val="0"/>
-          <c:showSerName val="0"/>
-          <c:showVal val="0"/>
-        </c:dLbls>
         <c:hiLowLines>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
+          <c:spPr>
             <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
         </c:hiLowLines>
-        <c:smooth val="0"/>
-        <c:axId val="37655487"/>
-        <c:axId val="33766647"/>
+        <c:marker val="0"/>
+        <c:axId val="55789895"/>
+        <c:axId val="96176429"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="37655487"/>
+        <c:axId val="55789895"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -483,32 +612,29 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
                   </a:rPr>
                   <a:t>Iterations</a:t>
                 </a:r>
-                <a:endParaRPr/>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
+          <c:spPr>
             <a:noFill/>
             <a:ln w="0">
               <a:noFill/>
@@ -519,13 +645,10 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr bwMode="auto">
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
+        <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="D9D9D9"/>
+              <a:srgbClr val="d9d9d9"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -535,17 +658,17 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Aptos Narrow"/>
+                <a:ea typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33766647"/>
+        <c:crossAx val="96176429"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -553,33 +676,27 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="33766647"/>
+        <c:axId val="96176429"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
+          <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="D9D9D9"/>
+                <a:srgbClr val="d9d9d9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
         <c:minorGridlines>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
+          <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="F2F2F2"/>
+                <a:srgbClr val="f2f2f2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -592,32 +709,29 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
                   </a:rPr>
                   <a:t>Seconds</a:t>
                 </a:r>
-                <a:endParaRPr/>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
+          <c:spPr>
             <a:noFill/>
             <a:ln w="0">
               <a:noFill/>
@@ -628,10 +742,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr bwMode="auto">
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
+        <c:spPr>
           <a:ln w="12600">
             <a:noFill/>
           </a:ln>
@@ -641,24 +752,21 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Aptos Narrow"/>
+                <a:ea typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37655487"/>
+        <c:crossAx val="55789895"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:spPr bwMode="auto">
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+      <c:spPr>
         <a:noFill/>
         <a:ln w="0">
           <a:noFill/>
@@ -667,12 +775,8 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
-      <c:spPr bwMode="auto">
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+      <c:spPr>
         <a:noFill/>
         <a:ln w="0">
           <a:noFill/>
@@ -683,60 +787,38 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+            <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="595959"/>
               </a:solidFill>
               <a:latin typeface="Aptos Narrow"/>
+              <a:ea typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="1"/>
   </c:chart>
-  <c:spPr bwMode="auto">
-    <a:xfrm>
-      <a:off x="0" y="0"/>
-      <a:ext cx="0" cy="0"/>
-    </a:xfrm>
-    <a:prstGeom prst="rect">
-      <a:avLst/>
-    </a:prstGeom>
+  <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
+      <a:srgbClr val="ffffff"/>
     </a:solidFill>
     <a:ln w="9360">
       <a:solidFill>
-        <a:srgbClr val="D9D9D9"/>
+        <a:srgbClr val="d9d9d9"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
   </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins l="0.69999999999999996" r="0.69999999999999996" t="0.75" b="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -745,32 +827,29 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr lang="en-US" sz="1400" b="0" strike="noStrike" spc="-1">
+              <a:defRPr b="0" lang="en-US" sz="1400" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Aptos Narrow"/>
+                <a:ea typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" strike="noStrike" spc="-1">
+              <a:rPr b="0" lang="en-US" sz="1400" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Aptos Narrow"/>
+                <a:ea typeface="Arial"/>
               </a:rPr>
               <a:t>x86 vs ARM Unoptimised</a:t>
             </a:r>
-            <a:endParaRPr/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
-      <c:spPr bwMode="auto">
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+      <c:spPr>
         <a:noFill/>
         <a:ln w="0">
           <a:noFill/>
@@ -779,7 +858,6 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -797,13 +875,13 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln w="28440" cap="rnd">
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="196b24"/>
+            </a:solidFill>
+            <a:ln cap="rnd" w="28440">
               <a:solidFill>
-                <a:srgbClr val="196B24"/>
+                <a:srgbClr val="196b24"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -812,40 +890,34 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
-            <c:dLblPos val="t"/>
-            <c:separator xml:space="preserve">; </c:separator>
-            <c:showBubbleSize val="1"/>
-            <c:showCatName val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:showLegendKey val="0"/>
-            <c:showPercent val="0"/>
-            <c:showSerName val="0"/>
-            <c:showVal val="0"/>
-            <c:spPr bwMode="auto">
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
@@ -890,7 +962,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.000045</c:v>
+                  <c:v>4.5E-005</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.076079</c:v>
@@ -920,13 +992,13 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln w="28440" cap="rnd">
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="0f9ed5"/>
+            </a:solidFill>
+            <a:ln cap="rnd" w="28440">
               <a:solidFill>
-                <a:srgbClr val="0F9ED5"/>
+                <a:srgbClr val="0f9ed5"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -935,40 +1007,34 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
-            <c:dLblPos val="t"/>
-            <c:separator xml:space="preserve">; </c:separator>
-            <c:showBubbleSize val="1"/>
-            <c:showCatName val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:showLegendKey val="0"/>
-            <c:showPercent val="0"/>
-            <c:showSerName val="0"/>
-            <c:showVal val="0"/>
-            <c:spPr bwMode="auto">
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
@@ -1013,7 +1079,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.000012</c:v>
+                  <c:v>1.2E-005</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.018605</c:v>
@@ -1029,31 +1095,19 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showBubbleSize val="0"/>
-          <c:showCatName val="0"/>
-          <c:showLeaderLines val="0"/>
-          <c:showLegendKey val="0"/>
-          <c:showPercent val="0"/>
-          <c:showSerName val="0"/>
-          <c:showVal val="0"/>
-        </c:dLbls>
         <c:hiLowLines>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
+          <c:spPr>
             <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
         </c:hiLowLines>
-        <c:smooth val="0"/>
-        <c:axId val="92450187"/>
-        <c:axId val="16042312"/>
+        <c:marker val="0"/>
+        <c:axId val="8531724"/>
+        <c:axId val="26314072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92450187"/>
+        <c:axId val="8531724"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1066,32 +1120,29 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-US" sz="800" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr b="0" lang="en-US" sz="800" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="800" b="0" strike="noStrike" spc="-1">
+                  <a:rPr b="0" lang="en-US" sz="800" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
                   </a:rPr>
                   <a:t>ITERATIONS</a:t>
                 </a:r>
-                <a:endParaRPr/>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
+          <c:spPr>
             <a:noFill/>
             <a:ln w="0">
               <a:noFill/>
@@ -1102,13 +1153,10 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr bwMode="auto">
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
+        <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="D9D9D9"/>
+              <a:srgbClr val="d9d9d9"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1118,17 +1166,17 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Aptos Narrow"/>
+                <a:ea typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16042312"/>
+        <c:crossAx val="26314072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1136,20 +1184,17 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="16042312"/>
+        <c:axId val="26314072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
+          <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="D9D9D9"/>
+                <a:srgbClr val="d9d9d9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1162,32 +1207,29 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-US" sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:rPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
                   </a:rPr>
                   <a:t>SECONDS</a:t>
                 </a:r>
-                <a:endParaRPr/>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
+          <c:spPr>
             <a:noFill/>
             <a:ln w="0">
               <a:noFill/>
@@ -1198,10 +1240,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr bwMode="auto">
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
+        <c:spPr>
           <a:ln w="12600">
             <a:noFill/>
           </a:ln>
@@ -1211,24 +1250,21 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Aptos Narrow"/>
+                <a:ea typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92450187"/>
+        <c:crossAx val="8531724"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:spPr bwMode="auto">
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+      <c:spPr>
         <a:noFill/>
         <a:ln w="0">
           <a:noFill/>
@@ -1237,12 +1273,8 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
-      <c:spPr bwMode="auto">
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+      <c:spPr>
         <a:noFill/>
         <a:ln w="0">
           <a:noFill/>
@@ -1253,60 +1285,38 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+            <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="595959"/>
               </a:solidFill>
               <a:latin typeface="Aptos Narrow"/>
+              <a:ea typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="1"/>
   </c:chart>
-  <c:spPr bwMode="auto">
-    <a:xfrm>
-      <a:off x="0" y="0"/>
-      <a:ext cx="0" cy="0"/>
-    </a:xfrm>
-    <a:prstGeom prst="rect">
-      <a:avLst/>
-    </a:prstGeom>
+  <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
+      <a:srgbClr val="ffffff"/>
     </a:solidFill>
     <a:ln w="9360">
       <a:solidFill>
-        <a:srgbClr val="D9D9D9"/>
+        <a:srgbClr val="d9d9d9"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
   </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins l="0.69999999999999996" r="0.69999999999999996" t="0.75" b="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1315,32 +1325,29 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr lang="en-US" sz="2000" b="0" strike="noStrike" spc="-1">
+              <a:defRPr b="0" lang="en-US" sz="2000" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Aptos Display"/>
+                <a:ea typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="2000" b="0" strike="noStrike" spc="-1">
+              <a:rPr b="0" lang="en-US" sz="2000" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Aptos Display"/>
+                <a:ea typeface="Arial"/>
               </a:rPr>
               <a:t>x86 vs ARM Unoptimised</a:t>
             </a:r>
-            <a:endParaRPr/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
-      <c:spPr bwMode="auto">
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+      <c:spPr>
         <a:noFill/>
         <a:ln w="0">
           <a:noFill/>
@@ -1349,7 +1356,6 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -1367,11 +1373,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln w="38160" cap="rnd">
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="156082"/>
+            </a:solidFill>
+            <a:ln cap="rnd" w="38160">
               <a:solidFill>
                 <a:srgbClr val="156082"/>
               </a:solidFill>
@@ -1382,40 +1388,34 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
-            <c:dLblPos val="r"/>
-            <c:separator xml:space="preserve">; </c:separator>
-            <c:showBubbleSize val="1"/>
-            <c:showCatName val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:showLegendKey val="0"/>
-            <c:showPercent val="0"/>
-            <c:showSerName val="0"/>
-            <c:showVal val="0"/>
-            <c:spPr bwMode="auto">
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
@@ -1460,7 +1460,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.000098</c:v>
+                  <c:v>9.8E-005</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.175177</c:v>
@@ -1468,7 +1468,7 @@
                 <c:pt idx="2">
                   <c:v>1.402216</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="#,##0.000000">
+                <c:pt idx="3">
                   <c:v>6.417753</c:v>
                 </c:pt>
               </c:numCache>
@@ -1490,13 +1490,13 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln w="38160" cap="rnd">
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="196b24"/>
+            </a:solidFill>
+            <a:ln cap="rnd" w="38160">
               <a:solidFill>
-                <a:srgbClr val="196B24"/>
+                <a:srgbClr val="196b24"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1505,40 +1505,34 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
-            <c:dLblPos val="r"/>
-            <c:separator xml:space="preserve">; </c:separator>
-            <c:showBubbleSize val="1"/>
-            <c:showCatName val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:showLegendKey val="0"/>
-            <c:showPercent val="0"/>
-            <c:showSerName val="0"/>
-            <c:showVal val="0"/>
-            <c:spPr bwMode="auto">
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
@@ -1583,7 +1577,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.000013</c:v>
+                  <c:v>1.3E-005</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.034103</c:v>
@@ -1591,7 +1585,7 @@
                 <c:pt idx="2">
                   <c:v>0.263528</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="#,##0.000000">
+                <c:pt idx="3">
                   <c:v>1.196854</c:v>
                 </c:pt>
               </c:numCache>
@@ -1599,31 +1593,19 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showBubbleSize val="0"/>
-          <c:showCatName val="0"/>
-          <c:showLeaderLines val="0"/>
-          <c:showLegendKey val="0"/>
-          <c:showPercent val="0"/>
-          <c:showSerName val="0"/>
-          <c:showVal val="0"/>
-        </c:dLbls>
         <c:hiLowLines>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
+          <c:spPr>
             <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
         </c:hiLowLines>
-        <c:smooth val="0"/>
-        <c:axId val="54063989"/>
-        <c:axId val="36264522"/>
+        <c:marker val="0"/>
+        <c:axId val="44559857"/>
+        <c:axId val="69757127"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="54063989"/>
+        <c:axId val="44559857"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1636,32 +1618,29 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
                   </a:rPr>
                   <a:t>ITERATIONS</a:t>
                 </a:r>
-                <a:endParaRPr/>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
+          <c:spPr>
             <a:noFill/>
             <a:ln w="0">
               <a:noFill/>
@@ -1672,13 +1651,10 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr bwMode="auto">
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
+        <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="D9D9D9"/>
+              <a:srgbClr val="d9d9d9"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1688,17 +1664,17 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Aptos Narrow"/>
+                <a:ea typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36264522"/>
+        <c:crossAx val="69757127"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1706,33 +1682,27 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="36264522"/>
+        <c:axId val="69757127"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
+          <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="D9D9D9"/>
+                <a:srgbClr val="d9d9d9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
         <c:minorGridlines>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
+          <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="F2F2F2"/>
+                <a:srgbClr val="f2f2f2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1745,32 +1715,29 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
                   </a:rPr>
                   <a:t>SECONDS</a:t>
                 </a:r>
-                <a:endParaRPr/>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
+          <c:spPr>
             <a:noFill/>
             <a:ln w="0">
               <a:noFill/>
@@ -1781,10 +1748,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr bwMode="auto">
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
+        <c:spPr>
           <a:ln w="12600">
             <a:noFill/>
           </a:ln>
@@ -1794,24 +1758,21 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Aptos Narrow"/>
+                <a:ea typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54063989"/>
+        <c:crossAx val="44559857"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:spPr bwMode="auto">
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+      <c:spPr>
         <a:noFill/>
         <a:ln w="0">
           <a:noFill/>
@@ -1820,12 +1781,8 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
-      <c:spPr bwMode="auto">
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+      <c:spPr>
         <a:noFill/>
         <a:ln w="0">
           <a:noFill/>
@@ -1836,60 +1793,38 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+            <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="595959"/>
               </a:solidFill>
               <a:latin typeface="Aptos Narrow"/>
+              <a:ea typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="1"/>
   </c:chart>
-  <c:spPr bwMode="auto">
-    <a:xfrm>
-      <a:off x="0" y="0"/>
-      <a:ext cx="0" cy="0"/>
-    </a:xfrm>
-    <a:prstGeom prst="rect">
-      <a:avLst/>
-    </a:prstGeom>
+  <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
+      <a:srgbClr val="ffffff"/>
     </a:solidFill>
     <a:ln w="9360">
       <a:solidFill>
-        <a:srgbClr val="D9D9D9"/>
+        <a:srgbClr val="d9d9d9"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
   </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins l="0.69999999999999996" r="0.69999999999999996" t="0.75" b="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1898,23 +1833,24 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr lang="en-US" sz="2000" b="0" strike="noStrike" spc="-1">
+              <a:defRPr b="0" lang="en-US" sz="2000" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Aptos Display"/>
+                <a:ea typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="2000" b="0" strike="noStrike" spc="-1">
+              <a:rPr b="0" lang="en-US" sz="2000" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Aptos Display"/>
+                <a:ea typeface="Arial"/>
               </a:rPr>
               <a:t>LSAL performance on ARM </a:t>
             </a:r>
-            <a:endParaRPr/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1922,15 +1858,12 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.430195"/>
-          <c:y val="0.028151"/>
+          <c:x val="0.430204767133906"/>
+          <c:y val="0.0281538159701785"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
-      <c:spPr bwMode="auto">
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+      <c:spPr>
         <a:noFill/>
         <a:ln w="0">
           <a:noFill/>
@@ -1939,7 +1872,6 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -1957,11 +1889,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln w="38160" cap="rnd">
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="156082"/>
+            </a:solidFill>
+            <a:ln cap="rnd" w="38160">
               <a:solidFill>
                 <a:srgbClr val="156082"/>
               </a:solidFill>
@@ -1972,40 +1904,34 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
-            <c:dLblPos val="r"/>
-            <c:separator xml:space="preserve">; </c:separator>
-            <c:showBubbleSize val="1"/>
-            <c:showCatName val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:showLegendKey val="0"/>
-            <c:showPercent val="0"/>
-            <c:showSerName val="0"/>
-            <c:showVal val="0"/>
-            <c:spPr bwMode="auto">
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
@@ -2050,7 +1976,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.000098</c:v>
+                  <c:v>9.8E-005</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.175177</c:v>
@@ -2058,7 +1984,7 @@
                 <c:pt idx="2">
                   <c:v>1.402216</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="#,##0.000000">
+                <c:pt idx="3">
                   <c:v>6.417753</c:v>
                 </c:pt>
               </c:numCache>
@@ -2080,13 +2006,13 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln w="38160" cap="rnd">
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="e97132"/>
+            </a:solidFill>
+            <a:ln cap="rnd" w="38160">
               <a:solidFill>
-                <a:srgbClr val="E97132"/>
+                <a:srgbClr val="e97132"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2095,40 +2021,34 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
-            <c:dLblPos val="r"/>
-            <c:separator xml:space="preserve">; </c:separator>
-            <c:showBubbleSize val="1"/>
-            <c:showCatName val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:showLegendKey val="0"/>
-            <c:showPercent val="0"/>
-            <c:showSerName val="0"/>
-            <c:showVal val="0"/>
-            <c:spPr bwMode="auto">
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
@@ -2173,7 +2093,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.000045</c:v>
+                  <c:v>4.5E-005</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.076079</c:v>
@@ -2189,31 +2109,19 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showBubbleSize val="0"/>
-          <c:showCatName val="0"/>
-          <c:showLeaderLines val="0"/>
-          <c:showLegendKey val="0"/>
-          <c:showPercent val="0"/>
-          <c:showSerName val="0"/>
-          <c:showVal val="0"/>
-        </c:dLbls>
         <c:hiLowLines>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
+          <c:spPr>
             <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
         </c:hiLowLines>
-        <c:smooth val="0"/>
-        <c:axId val="10855597"/>
-        <c:axId val="79791227"/>
+        <c:marker val="0"/>
+        <c:axId val="23817325"/>
+        <c:axId val="56040951"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="10855597"/>
+        <c:axId val="23817325"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2226,32 +2134,29 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
                   </a:rPr>
                   <a:t>ITERATIONS</a:t>
                 </a:r>
-                <a:endParaRPr/>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
+          <c:spPr>
             <a:noFill/>
             <a:ln w="0">
               <a:noFill/>
@@ -2262,13 +2167,10 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr bwMode="auto">
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
+        <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="D9D9D9"/>
+              <a:srgbClr val="d9d9d9"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -2278,17 +2180,17 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Aptos Narrow"/>
+                <a:ea typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79791227"/>
+        <c:crossAx val="56040951"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2296,33 +2198,27 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79791227"/>
+        <c:axId val="56040951"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
+          <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="D9D9D9"/>
+                <a:srgbClr val="d9d9d9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
         <c:minorGridlines>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
+          <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="F2F2F2"/>
+                <a:srgbClr val="f2f2f2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2335,32 +2231,29 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
                     <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
                   </a:rPr>
                   <a:t>SECONDS</a:t>
                 </a:r>
-                <a:endParaRPr/>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
+          <c:spPr>
             <a:noFill/>
             <a:ln w="0">
               <a:noFill/>
@@ -2371,10 +2264,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr bwMode="auto">
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
+        <c:spPr>
           <a:ln w="12600">
             <a:noFill/>
           </a:ln>
@@ -2384,24 +2274,21 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Aptos Narrow"/>
+                <a:ea typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10855597"/>
+        <c:crossAx val="23817325"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:spPr bwMode="auto">
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+      <c:spPr>
         <a:noFill/>
         <a:ln w="0">
           <a:noFill/>
@@ -2410,12 +2297,8 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
-      <c:spPr bwMode="auto">
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+      <c:spPr>
         <a:noFill/>
         <a:ln w="0">
           <a:noFill/>
@@ -2426,72 +2309,57 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+            <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="595959"/>
               </a:solidFill>
               <a:latin typeface="Aptos Narrow"/>
+              <a:ea typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="1"/>
   </c:chart>
-  <c:spPr bwMode="auto">
-    <a:xfrm>
-      <a:off x="0" y="0"/>
-      <a:ext cx="0" cy="0"/>
-    </a:xfrm>
-    <a:prstGeom prst="rect">
-      <a:avLst/>
-    </a:prstGeom>
+  <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
+      <a:srgbClr val="ffffff"/>
     </a:solidFill>
     <a:ln w="9360">
       <a:solidFill>
-        <a:srgbClr val="D9D9D9"/>
+        <a:srgbClr val="d9d9d9"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
   </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins l="0.69999999999999996" r="0.69999999999999996" t="0.75" b="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>38160</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>7559</xdr:rowOff>
+      <xdr:rowOff>7560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>30239</xdr:colOff>
+      <xdr:colOff>29880</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>14760</xdr:rowOff>
+      <xdr:rowOff>14400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Γράφημα 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvPr id="0" name="Γράφημα 1"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off x="38160" y="1245960"/>
+        <a:ext cx="9867240" cy="3807000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2510,20 +2378,18 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>88560</xdr:colOff>
+      <xdr:colOff>88200</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>113760</xdr:rowOff>
+      <xdr:rowOff>113400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Γράφημα 3"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvPr id="1" name="Γράφημα 3"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off x="0" y="6883200"/>
+        <a:ext cx="9963720" cy="3850560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2542,20 +2408,18 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>37440</xdr:colOff>
+      <xdr:colOff>37080</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>24839</xdr:rowOff>
+      <xdr:rowOff>24480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 4"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off x="11923920" y="6721200"/>
+        <a:ext cx="11656440" cy="4104720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2574,20 +2438,18 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>2996999</xdr:colOff>
+      <xdr:colOff>2996640</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>139320</xdr:rowOff>
+      <xdr:rowOff>138960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 5"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off x="11905200" y="1327320"/>
+        <a:ext cx="11145960" cy="3669480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2606,23 +2468,23 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>30239</xdr:colOff>
+      <xdr:colOff>29880</xdr:colOff>
       <xdr:row>122</xdr:row>
-      <xdr:rowOff>43560</xdr:rowOff>
+      <xdr:rowOff>43200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Image 1"/>
+        <xdr:cNvPr id="4" name="Image 1" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId5"/>
         <a:stretch/>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="322560" y="11111400"/>
-          <a:ext cx="23260320" cy="11373120"/>
+          <a:off x="322560" y="11054160"/>
+          <a:ext cx="23250600" cy="11372760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2638,7 +2500,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Πίνακας1" ref="A2:E6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:E6" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A2:E6"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Ν"/>
@@ -2647,12 +2509,11 @@
     <tableColumn id="4" name="optimised (s)"/>
     <tableColumn id="5" name="Optimisation"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" displayName="Πίνακας13" ref="I2:M6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Πίνακας13" displayName="Πίνακας13" ref="I2:M6" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="I2:M6"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Ν"/>
@@ -2661,12 +2522,11 @@
     <tableColumn id="4" name="optimised (s)"/>
     <tableColumn id="5" name="Optimisation"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" displayName="Πίνακας14" ref="A31:E35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Πίνακας14" displayName="Πίνακας14" ref="A31:E35" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A31:E35"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Ν"/>
@@ -2675,12 +2535,11 @@
     <tableColumn id="4" name="x86"/>
     <tableColumn id="5" name="Optimisation"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" displayName="Πίνακας145" ref="I31:M35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Πίνακας145" displayName="Πίνακας145" ref="I31:M35" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="I31:M35"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Ν"/>
@@ -2689,12 +2548,11 @@
     <tableColumn id="4" name="x86"/>
     <tableColumn id="5" name="Optimisation"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" displayName="Πίνακας16" ref="Q2:U7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Πίνακας16" displayName="Πίνακας16" ref="Q2:U7" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="Q2:U7"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Ν"/>
@@ -2703,347 +2561,63 @@
     <tableColumn id="4" name="optimised (s)"/>
     <tableColumn id="5" name="Optimisation"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="0e2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Angsana New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Cordia New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="0E2841"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="e8e8e8"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="e97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="196b24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="0f9ed5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="a02b93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="4ea72e"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="96607d"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Aptos Display" pitchFamily="0" charset="1"/>
+        <a:ea typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:cs typeface="Arial" pitchFamily="0" charset="1"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Aptos Narrow" pitchFamily="0" charset="1"/>
+        <a:ea typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:cs typeface="Arial" pitchFamily="0" charset="1"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme>
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3053,39 +2627,35 @@
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
                 <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
                 <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
                 <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
                 <a:lumMod val="102000"/>
                 <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
                 <a:lumMod val="100000"/>
                 <a:shade val="100000"/>
               </a:schemeClr>
@@ -3093,64 +2663,37 @@
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
                 <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -3160,7 +2703,6 @@
         <a:solidFill>
           <a:schemeClr val="phClr">
             <a:tint val="95000"/>
-            <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:gradFill>
@@ -3168,7 +2710,6 @@
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="93000"/>
-                <a:satMod val="150000"/>
                 <a:shade val="98000"/>
                 <a:lumMod val="102000"/>
               </a:schemeClr>
@@ -3176,7 +2717,6 @@
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:tint val="98000"/>
-                <a:satMod val="130000"/>
                 <a:shade val="90000"/>
                 <a:lumMod val="103000"/>
               </a:schemeClr>
@@ -3184,66 +2724,49 @@
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="63000"/>
-                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr bwMode="auto"/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView zoomScale="70" workbookViewId="0">
-      <selection activeCell="Q11" activeCellId="0" sqref="Q11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S27" activeCellId="0" sqref="S27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="19.77734375"/>
-    <col customWidth="1" min="2" max="2" width="23.33203125"/>
-    <col customWidth="1" min="3" max="3" width="24.21875"/>
-    <col customWidth="1" min="4" max="4" width="30.21875"/>
-    <col customWidth="1" min="5" max="5" width="28.88671875"/>
-    <col customWidth="1" min="9" max="9" width="26.77734375"/>
-    <col customWidth="1" min="10" max="10" width="25.6640625"/>
-    <col customWidth="1" min="11" max="11" width="29.21875"/>
-    <col customWidth="1" min="12" max="12" width="23"/>
-    <col customWidth="1" min="13" max="13" width="44.6640625"/>
-    <col customWidth="1" min="17" max="17" width="16.88671875"/>
-    <col customWidth="1" min="18" max="18" width="20.6640625"/>
-    <col customWidth="1" min="19" max="19" width="22.77734375"/>
-    <col customWidth="1" min="20" max="20" width="27.44140625"/>
-    <col customWidth="1" min="21" max="21" width="26.109375"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="29.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="44.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="16.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="20.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="22.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="27.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="26.11"/>
   </cols>
   <sheetData>
-    <row r="1" ht="26.25">
+    <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3266,7 +2789,7 @@
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -3313,200 +2836,200 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="2">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="C3" s="2">
-        <v>1.2999999999999999e-05</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1.2e-05</v>
-      </c>
-      <c r="E3" s="3">
-        <f t="shared" ref="E3:E6" si="0">D3/C3</f>
-        <v>0.92307692307692313</v>
-      </c>
-      <c r="I3" s="2">
+      <c r="C3" s="3" t="n">
+        <v>1.3E-005</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>1.2E-005</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <f aca="false">D3/C3</f>
+        <v>0.923076923076923</v>
+      </c>
+      <c r="I3" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="K3" s="2">
-        <v>9.7999999999999997e-05</v>
-      </c>
-      <c r="L3" s="2">
-        <v>4.5000000000000003e-05</v>
-      </c>
-      <c r="M3" s="3">
-        <f t="shared" ref="M3:M6" si="1">L3/K3</f>
-        <v>0.45918367346938782</v>
-      </c>
-      <c r="Q3" s="2">
+      <c r="K3" s="3" t="n">
+        <v>9.8E-005</v>
+      </c>
+      <c r="L3" s="3" t="n">
+        <v>4.5E-005</v>
+      </c>
+      <c r="M3" s="4" t="n">
+        <f aca="false">L3/K3</f>
+        <v>0.459183673469388</v>
+      </c>
+      <c r="Q3" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="R3" s="2">
+      <c r="R3" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="S3" s="2">
-        <v>0.0025655640000000002</v>
-      </c>
-      <c r="T3" s="2"/>
-      <c r="U3" s="3">
-        <f t="shared" ref="U3:U5" si="2">T3/S3</f>
+      <c r="S3" s="3" t="n">
+        <v>0.002565564</v>
+      </c>
+      <c r="T3" s="3"/>
+      <c r="U3" s="4" t="n">
+        <f aca="false">T3/S3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="2">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3" t="n">
         <v>65536</v>
       </c>
-      <c r="C4" s="2">
-        <v>0.034103000000000001</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="C4" s="3" t="n">
+        <v>0.034103</v>
+      </c>
+      <c r="D4" s="3" t="n">
         <v>0.018605</v>
       </c>
-      <c r="E4" s="3">
-        <f t="shared" si="0"/>
-        <v>0.54555317713984108</v>
-      </c>
-      <c r="I4" s="2">
+      <c r="E4" s="4" t="n">
+        <f aca="false">D4/C4</f>
+        <v>0.545553177139841</v>
+      </c>
+      <c r="I4" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="3" t="n">
         <v>65536</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="3" t="n">
         <v>0.175177</v>
       </c>
-      <c r="L4" s="2">
-        <v>0.076078999999999994</v>
-      </c>
-      <c r="M4" s="3">
-        <f t="shared" si="1"/>
-        <v>0.4342978815712108</v>
-      </c>
-      <c r="Q4" s="2">
+      <c r="L4" s="3" t="n">
+        <v>0.076079</v>
+      </c>
+      <c r="M4" s="4" t="n">
+        <f aca="false">L4/K4</f>
+        <v>0.434297881571211</v>
+      </c>
+      <c r="Q4" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="R4" s="2">
+      <c r="R4" s="3" t="n">
         <v>65536</v>
       </c>
-      <c r="S4" s="2">
-        <v>2.6276989529999999</v>
-      </c>
-      <c r="T4" s="2"/>
-      <c r="U4" s="3">
-        <f t="shared" si="2"/>
+      <c r="S4" s="3" t="n">
+        <v>3.268688927</v>
+      </c>
+      <c r="T4" s="3"/>
+      <c r="U4" s="4" t="n">
+        <f aca="false">T4/S4</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="2">
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="n">
         <v>256</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3" t="n">
         <v>65536</v>
       </c>
-      <c r="C5" s="2">
-        <v>0.26352799999999998</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0.13781299999999999</v>
-      </c>
-      <c r="E5" s="3">
-        <f t="shared" si="0"/>
-        <v>0.52295391761027288</v>
-      </c>
-      <c r="I5" s="2">
+      <c r="C5" s="3" t="n">
+        <v>0.263528</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>0.137813</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <f aca="false">D5/C5</f>
+        <v>0.522953917610273</v>
+      </c>
+      <c r="I5" s="3" t="n">
         <v>256</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="3" t="n">
         <v>65536</v>
       </c>
-      <c r="K5" s="2">
-        <v>1.4022159999999999</v>
-      </c>
-      <c r="L5" s="2">
-        <v>0.58648800000000001</v>
-      </c>
-      <c r="M5" s="3">
-        <f t="shared" si="1"/>
-        <v>0.41825795740456539</v>
-      </c>
-      <c r="Q5" s="2">
+      <c r="K5" s="3" t="n">
+        <v>1.402216</v>
+      </c>
+      <c r="L5" s="3" t="n">
+        <v>0.586488</v>
+      </c>
+      <c r="M5" s="4" t="n">
+        <f aca="false">L5/K5</f>
+        <v>0.418257957404565</v>
+      </c>
+      <c r="Q5" s="3" t="n">
         <v>256</v>
       </c>
-      <c r="R5" s="2">
+      <c r="R5" s="3" t="n">
         <v>65536</v>
       </c>
-      <c r="S5" s="2">
-        <v>0.44895658399999999</v>
-      </c>
-      <c r="T5" s="2"/>
-      <c r="U5" s="3">
-        <f t="shared" si="2"/>
+      <c r="S5" s="3" t="n">
+        <v>0.443408594</v>
+      </c>
+      <c r="T5" s="3"/>
+      <c r="U5" s="4" t="n">
+        <f aca="false">T5/S5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="2">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="n">
         <v>256</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3" t="n">
         <v>300000</v>
       </c>
-      <c r="C6" s="4">
-        <v>1.1968540000000001</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0.62857499999999999</v>
-      </c>
-      <c r="E6" s="3">
-        <f t="shared" si="0"/>
-        <v>0.52518937146886746</v>
-      </c>
-      <c r="I6" s="2">
+      <c r="C6" s="5" t="n">
+        <v>1.196854</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>0.628575</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <f aca="false">D6/C6</f>
+        <v>0.525189371468868</v>
+      </c>
+      <c r="I6" s="3" t="n">
         <v>256</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="3" t="n">
         <v>300000</v>
       </c>
-      <c r="K6" s="4">
-        <v>6.4177530000000003</v>
-      </c>
-      <c r="L6" s="2">
-        <v>2.6851039999999999</v>
-      </c>
-      <c r="M6" s="3">
-        <f t="shared" si="1"/>
-        <v>0.41838693386922182</v>
-      </c>
-      <c r="Q6" s="2">
+      <c r="K6" s="5" t="n">
+        <v>6.417753</v>
+      </c>
+      <c r="L6" s="3" t="n">
+        <v>2.685104</v>
+      </c>
+      <c r="M6" s="4" t="n">
+        <f aca="false">L6/K6</f>
+        <v>0.418386933869222</v>
+      </c>
+      <c r="Q6" s="3" t="n">
         <v>256</v>
       </c>
-      <c r="R6" s="2">
+      <c r="R6" s="3" t="n">
         <v>300000</v>
       </c>
-      <c r="S6" s="5" t="s">
+      <c r="S6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="T6" s="6" t="s">
+      <c r="T6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="U6" s="7" t="s">
+      <c r="U6" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" ht="26.25">
+    <row r="30" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>9</v>
       </c>
@@ -3522,7 +3045,7 @@
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
     </row>
-    <row r="31">
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
         <v>3</v>
       </c>
@@ -3554,140 +3077,140 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="2">
+    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="C32" s="2">
-        <v>4.5000000000000003e-05</v>
-      </c>
-      <c r="D32" s="2">
-        <v>1.2e-05</v>
-      </c>
-      <c r="E32" s="3">
-        <f t="shared" ref="E32:E35" si="3">D32/C32</f>
-        <v>0.26666666666666666</v>
-      </c>
-      <c r="I32" s="2">
+      <c r="C32" s="3" t="n">
+        <v>4.5E-005</v>
+      </c>
+      <c r="D32" s="3" t="n">
+        <v>1.2E-005</v>
+      </c>
+      <c r="E32" s="4" t="n">
+        <f aca="false">D32/C32</f>
+        <v>0.266666666666667</v>
+      </c>
+      <c r="I32" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="J32" s="2">
+      <c r="J32" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="K32" s="2">
-        <v>9.7999999999999997e-05</v>
-      </c>
-      <c r="L32" s="2">
-        <v>1.2999999999999999e-05</v>
-      </c>
-      <c r="M32" s="3">
-        <f t="shared" ref="M32:M35" si="4">L32/K32</f>
-        <v>0.1326530612244898</v>
+      <c r="K32" s="3" t="n">
+        <v>9.8E-005</v>
+      </c>
+      <c r="L32" s="3" t="n">
+        <v>1.3E-005</v>
+      </c>
+      <c r="M32" s="4" t="n">
+        <f aca="false">L32/K32</f>
+        <v>0.13265306122449</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="2">
+    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="3" t="n">
         <v>65536</v>
       </c>
-      <c r="C33" s="2">
-        <v>0.076078999999999994</v>
-      </c>
-      <c r="D33" s="2">
+      <c r="C33" s="3" t="n">
+        <v>0.076079</v>
+      </c>
+      <c r="D33" s="3" t="n">
         <v>0.018605</v>
       </c>
-      <c r="E33" s="3">
-        <f t="shared" si="3"/>
-        <v>0.24454842992152895</v>
-      </c>
-      <c r="I33" s="2">
+      <c r="E33" s="4" t="n">
+        <f aca="false">D33/C33</f>
+        <v>0.244548429921529</v>
+      </c>
+      <c r="I33" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="J33" s="2">
+      <c r="J33" s="3" t="n">
         <v>65536</v>
       </c>
-      <c r="K33" s="2">
+      <c r="K33" s="3" t="n">
         <v>0.175177</v>
       </c>
-      <c r="L33" s="2">
-        <v>0.034103000000000001</v>
-      </c>
-      <c r="M33" s="3">
-        <f t="shared" si="4"/>
-        <v>0.19467738344645702</v>
+      <c r="L33" s="3" t="n">
+        <v>0.034103</v>
+      </c>
+      <c r="M33" s="4" t="n">
+        <f aca="false">L33/K33</f>
+        <v>0.194677383446457</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" s="2">
+    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3" t="n">
         <v>256</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="3" t="n">
         <v>65536</v>
       </c>
-      <c r="C34" s="2">
-        <v>0.58648800000000001</v>
-      </c>
-      <c r="D34" s="2">
-        <v>0.13781299999999999</v>
-      </c>
-      <c r="E34" s="3">
-        <f t="shared" si="3"/>
-        <v>0.23498008484402066</v>
-      </c>
-      <c r="I34" s="2">
+      <c r="C34" s="3" t="n">
+        <v>0.586488</v>
+      </c>
+      <c r="D34" s="3" t="n">
+        <v>0.137813</v>
+      </c>
+      <c r="E34" s="4" t="n">
+        <f aca="false">D34/C34</f>
+        <v>0.234980084844021</v>
+      </c>
+      <c r="I34" s="3" t="n">
         <v>256</v>
       </c>
-      <c r="J34" s="2">
+      <c r="J34" s="3" t="n">
         <v>65536</v>
       </c>
-      <c r="K34" s="2">
-        <v>1.4022159999999999</v>
-      </c>
-      <c r="L34" s="2">
-        <v>0.26352799999999998</v>
-      </c>
-      <c r="M34" s="3">
-        <f t="shared" si="4"/>
-        <v>0.18793680859439629</v>
+      <c r="K34" s="3" t="n">
+        <v>1.402216</v>
+      </c>
+      <c r="L34" s="3" t="n">
+        <v>0.263528</v>
+      </c>
+      <c r="M34" s="4" t="n">
+        <f aca="false">L34/K34</f>
+        <v>0.187936808594396</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="2">
+    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="3" t="n">
         <v>256</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35" s="3" t="n">
         <v>300000</v>
       </c>
-      <c r="C35" s="2">
-        <v>2.6851039999999999</v>
-      </c>
-      <c r="D35" s="2">
-        <v>0.62857499999999999</v>
-      </c>
-      <c r="E35" s="3">
-        <f t="shared" si="3"/>
-        <v>0.23409707780406272</v>
-      </c>
-      <c r="I35" s="2">
+      <c r="C35" s="3" t="n">
+        <v>2.685104</v>
+      </c>
+      <c r="D35" s="3" t="n">
+        <v>0.628575</v>
+      </c>
+      <c r="E35" s="4" t="n">
+        <f aca="false">D35/C35</f>
+        <v>0.234097077804063</v>
+      </c>
+      <c r="I35" s="3" t="n">
         <v>256</v>
       </c>
-      <c r="J35" s="2">
+      <c r="J35" s="3" t="n">
         <v>300000</v>
       </c>
-      <c r="K35" s="4">
-        <v>6.4177530000000003</v>
-      </c>
-      <c r="L35" s="4">
-        <v>1.1968540000000001</v>
-      </c>
-      <c r="M35" s="3">
-        <f t="shared" si="4"/>
-        <v>0.18649112859282682</v>
+      <c r="K35" s="5" t="n">
+        <v>6.417753</v>
+      </c>
+      <c r="L35" s="5" t="n">
+        <v>1.196854</v>
+      </c>
+      <c r="M35" s="4" t="n">
+        <f aca="false">L35/K35</f>
+        <v>0.186491128592827</v>
       </c>
     </row>
   </sheetData>
@@ -3698,12 +3221,15 @@
     <mergeCell ref="A30:E30"/>
     <mergeCell ref="I30:M30"/>
   </mergeCells>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.51181102362204689" footer="0.51181102362204689"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
   <drawing r:id="rId1"/>
-  <tableParts count="5">
+  <tableParts>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>

</xml_diff>

<commit_message>
added correct values in sw after changes
</commit_message>
<xml_diff>
--- a/lab3/lsal/lab3 LSAL imlementation.xlsx
+++ b/lab3/lsal/lab3 LSAL imlementation.xlsx
@@ -1,17 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sstat\Documents\GitHub\Embedded-Systems\lab3\lsal\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13449057-7542-4342-87B0-4497DD571751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Φύλλο1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Φύλλο1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -20,110 +36,73 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="13">
   <si>
-    <t xml:space="preserve">x86</t>
+    <t>x86</t>
   </si>
   <si>
-    <t xml:space="preserve">ARM</t>
+    <t>ARM</t>
   </si>
   <si>
-    <t xml:space="preserve">FPGA</t>
+    <t>FPGA</t>
   </si>
   <si>
-    <t xml:space="preserve">Ν</t>
+    <t>Ν</t>
   </si>
   <si>
-    <t xml:space="preserve">Μ</t>
+    <t>Μ</t>
   </si>
   <si>
-    <t xml:space="preserve">unoptimised (s)</t>
+    <t>unoptimised (s)</t>
   </si>
   <si>
-    <t xml:space="preserve">optimised (s)</t>
+    <t>optimised (s)</t>
   </si>
   <si>
-    <t xml:space="preserve">Optimisation</t>
+    <t>Optimisation</t>
   </si>
   <si>
-    <t xml:space="preserve">-</t>
+    <t>-</t>
   </si>
   <si>
-    <t xml:space="preserve">x86 vs ARM Optimized</t>
+    <t>x86 vs ARM Optimized</t>
   </si>
   <si>
-    <t xml:space="preserve">x86 vs ARM Unoptimized</t>
+    <t>x86 vs ARM Unoptimized</t>
+  </si>
+  <si>
+    <t>sol 1</t>
+  </si>
+  <si>
+    <t>sol 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.0000%"/>
-    <numFmt numFmtId="166" formatCode="#,##0.000000"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0000%"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000000"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="22"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="20"/>
-      <color rgb="FF595959"/>
-      <name val="Aptos Display"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF595959"/>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF595959"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF595959"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF595959"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -141,113 +120,110 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="10">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -306,15 +282,33 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -323,7 +317,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" lang="en-US" sz="2000" spc="-1" strike="noStrike">
+              <a:defRPr lang="en-US" sz="2000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -332,7 +326,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" lang="en-US" sz="2000" spc="-1" strike="noStrike">
+              <a:rPr lang="en-US" sz="2000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -354,6 +348,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -372,12 +367,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="196b24"/>
-            </a:solidFill>
-            <a:ln cap="rnd" w="38160">
+            <a:ln w="38160" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="196b24"/>
+                <a:srgbClr val="196B24"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -386,12 +378,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -399,6 +398,7 @@
                     <a:ea typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -407,6 +407,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
             <c:extLst>
@@ -458,21 +459,26 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.3E-005</c:v>
+                  <c:v>2.0000000000000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.034103</c:v>
+                  <c:v>3.7108000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.263528</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.196854</c:v>
+                  <c:v>0.30333500000000002</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="#,##0.000000">
+                  <c:v>1.3882559999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4ABE-42CB-9CAB-7AAA5586332A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -489,12 +495,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="0f9ed5"/>
-            </a:solidFill>
-            <a:ln cap="rnd" w="38160">
+            <a:ln w="38160" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="0f9ed5"/>
+                <a:srgbClr val="0F9ED5"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -503,12 +506,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -516,6 +526,7 @@
                     <a:ea typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -524,6 +535,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
             <c:extLst>
@@ -575,22 +587,35 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.2E-005</c:v>
+                  <c:v>1.5E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.018605</c:v>
+                  <c:v>2.4056999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.137813</c:v>
+                  <c:v>0.19692599999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.628575</c:v>
+                  <c:v>0.89723900000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4ABE-42CB-9CAB-7AAA5586332A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
             <a:ln w="0">
@@ -598,7 +623,7 @@
             </a:ln>
           </c:spPr>
         </c:hiLowLines>
-        <c:marker val="0"/>
+        <c:smooth val="0"/>
         <c:axId val="59955241"/>
         <c:axId val="59010794"/>
       </c:lineChart>
@@ -616,7 +641,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -625,7 +650,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -652,7 +677,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
+              <a:srgbClr val="D9D9D9"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -662,7 +687,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -670,6 +695,7 @@
                 <a:ea typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="59010794"/>
@@ -690,7 +716,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -700,7 +726,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="f2f2f2"/>
+                <a:srgbClr val="F2F2F2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -713,7 +739,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -722,7 +748,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -756,7 +782,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -764,6 +790,7 @@
                 <a:ea typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="59955241"/>
@@ -791,7 +818,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+            <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
               <a:solidFill>
                 <a:srgbClr val="595959"/>
               </a:solidFill>
@@ -799,30 +826,39 @@
               <a:ea typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln w="9360">
       <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
+        <a:srgbClr val="D9D9D9"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -831,7 +867,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" lang="en-US" sz="1400" spc="-1" strike="noStrike">
+              <a:defRPr lang="en-US" sz="1400" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -840,7 +876,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" lang="en-US" sz="1400" spc="-1" strike="noStrike">
+              <a:rPr lang="en-US" sz="1400" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -862,6 +898,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -880,12 +917,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="196b24"/>
-            </a:solidFill>
-            <a:ln cap="rnd" w="28440">
+            <a:ln w="28440" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="196b24"/>
+                <a:srgbClr val="196B24"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -894,12 +928,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -907,6 +948,7 @@
                     <a:ea typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -915,6 +957,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
             <c:extLst>
@@ -966,21 +1009,26 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4.5E-005</c:v>
+                  <c:v>4.5000000000000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.076079</c:v>
+                  <c:v>7.6078999999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.586488</c:v>
+                  <c:v>0.58648800000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.685104</c:v>
+                  <c:v>2.6851039999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FF9E-4771-A7D6-5E773E4771CB}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -997,12 +1045,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="0f9ed5"/>
-            </a:solidFill>
-            <a:ln cap="rnd" w="28440">
+            <a:ln w="28440" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="0f9ed5"/>
+                <a:srgbClr val="0F9ED5"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1011,12 +1056,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1024,6 +1076,7 @@
                     <a:ea typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -1032,6 +1085,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
             <c:extLst>
@@ -1083,22 +1137,35 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.2E-005</c:v>
+                  <c:v>1.5E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.018605</c:v>
+                  <c:v>2.4056999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.137813</c:v>
+                  <c:v>0.19692599999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.628575</c:v>
+                  <c:v>0.89723900000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FF9E-4771-A7D6-5E773E4771CB}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
             <a:ln w="0">
@@ -1106,7 +1173,7 @@
             </a:ln>
           </c:spPr>
         </c:hiLowLines>
-        <c:marker val="0"/>
+        <c:smooth val="0"/>
         <c:axId val="6360646"/>
         <c:axId val="93816331"/>
       </c:lineChart>
@@ -1124,7 +1191,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="800" spc="-1" strike="noStrike">
+                  <a:defRPr lang="en-US" sz="800" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1133,7 +1200,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" lang="en-US" sz="800" spc="-1" strike="noStrike">
+                  <a:rPr lang="en-US" sz="800" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1160,7 +1227,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
+              <a:srgbClr val="D9D9D9"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1170,7 +1237,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1178,6 +1245,7 @@
                 <a:ea typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="93816331"/>
@@ -1198,7 +1266,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1211,7 +1279,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr lang="en-US" sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1220,7 +1288,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" lang="en-US" sz="1000" spc="-1" strike="noStrike">
+                  <a:rPr lang="en-US" sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1254,7 +1322,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1262,6 +1330,7 @@
                 <a:ea typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="6360646"/>
@@ -1289,7 +1358,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+            <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
               <a:solidFill>
                 <a:srgbClr val="595959"/>
               </a:solidFill>
@@ -1297,30 +1366,39 @@
               <a:ea typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln w="9360">
       <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
+        <a:srgbClr val="D9D9D9"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1329,7 +1407,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" lang="en-US" sz="2000" spc="-1" strike="noStrike">
+              <a:defRPr lang="en-US" sz="2000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1338,7 +1416,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" lang="en-US" sz="2000" spc="-1" strike="noStrike">
+              <a:rPr lang="en-US" sz="2000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1360,6 +1438,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -1378,10 +1457,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="156082"/>
-            </a:solidFill>
-            <a:ln cap="rnd" w="38160">
+            <a:ln w="38160" cap="rnd">
               <a:solidFill>
                 <a:srgbClr val="156082"/>
               </a:solidFill>
@@ -1392,12 +1468,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1405,6 +1488,7 @@
                     <a:ea typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -1413,6 +1497,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
             <c:extLst>
@@ -1464,21 +1549,26 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>9.8E-005</c:v>
+                  <c:v>9.7999999999999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.175177</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.402216</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.417753</c:v>
+                  <c:v>1.4022159999999999</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="#,##0.000000">
+                  <c:v>6.4177530000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9CE0-4BF4-988A-8048AB495EF6}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1495,12 +1585,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="196b24"/>
-            </a:solidFill>
-            <a:ln cap="rnd" w="38160">
+            <a:ln w="38160" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="196b24"/>
+                <a:srgbClr val="196B24"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1509,12 +1596,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1522,6 +1616,7 @@
                     <a:ea typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -1530,6 +1625,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
             <c:extLst>
@@ -1581,22 +1677,35 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.3E-005</c:v>
+                  <c:v>2.0000000000000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.034103</c:v>
+                  <c:v>3.7108000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.263528</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.196854</c:v>
+                  <c:v>0.30333500000000002</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="#,##0.000000">
+                  <c:v>1.3882559999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9CE0-4BF4-988A-8048AB495EF6}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
             <a:ln w="0">
@@ -1604,7 +1713,7 @@
             </a:ln>
           </c:spPr>
         </c:hiLowLines>
-        <c:marker val="0"/>
+        <c:smooth val="0"/>
         <c:axId val="81296340"/>
         <c:axId val="68456133"/>
       </c:lineChart>
@@ -1622,7 +1731,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1631,7 +1740,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1658,7 +1767,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
+              <a:srgbClr val="D9D9D9"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1668,7 +1777,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1676,6 +1785,7 @@
                 <a:ea typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="68456133"/>
@@ -1696,7 +1806,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1706,7 +1816,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="f2f2f2"/>
+                <a:srgbClr val="F2F2F2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1719,7 +1829,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1728,7 +1838,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1762,7 +1872,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1770,6 +1880,7 @@
                 <a:ea typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="81296340"/>
@@ -1797,7 +1908,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+            <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
               <a:solidFill>
                 <a:srgbClr val="595959"/>
               </a:solidFill>
@@ -1805,30 +1916,39 @@
               <a:ea typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln w="9360">
       <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
+        <a:srgbClr val="D9D9D9"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1837,7 +1957,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" lang="en-US" sz="2000" spc="-1" strike="noStrike">
+              <a:defRPr lang="en-US" sz="2000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1846,7 +1966,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" lang="en-US" sz="2000" spc="-1" strike="noStrike">
+              <a:rPr lang="en-US" sz="2000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1862,8 +1982,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.430218662187914"/>
-          <c:y val="0.0281565780437555"/>
+          <c:x val="0.43021866218791399"/>
+          <c:y val="2.8156578043755501E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1876,6 +1996,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -1894,10 +2015,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="156082"/>
-            </a:solidFill>
-            <a:ln cap="rnd" w="38160">
+            <a:ln w="38160" cap="rnd">
               <a:solidFill>
                 <a:srgbClr val="156082"/>
               </a:solidFill>
@@ -1908,12 +2026,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1921,6 +2046,7 @@
                     <a:ea typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -1929,6 +2055,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
             <c:extLst>
@@ -1980,21 +2107,26 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>9.8E-005</c:v>
+                  <c:v>9.7999999999999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.175177</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.402216</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.417753</c:v>
+                  <c:v>1.4022159999999999</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="#,##0.000000">
+                  <c:v>6.4177530000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-50F7-4DC0-B48F-FA3220C5C93D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2011,12 +2143,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="e97132"/>
-            </a:solidFill>
-            <a:ln cap="rnd" w="38160">
+            <a:ln w="38160" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="e97132"/>
+                <a:srgbClr val="E97132"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2025,12 +2154,19 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -2038,6 +2174,7 @@
                     <a:ea typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -2046,6 +2183,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
             <c:extLst>
@@ -2097,22 +2235,35 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4.5E-005</c:v>
+                  <c:v>4.5000000000000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.076079</c:v>
+                  <c:v>7.6078999999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.586488</c:v>
+                  <c:v>0.58648800000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.685104</c:v>
+                  <c:v>2.6851039999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-50F7-4DC0-B48F-FA3220C5C93D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
             <a:ln w="0">
@@ -2120,7 +2271,7 @@
             </a:ln>
           </c:spPr>
         </c:hiLowLines>
-        <c:marker val="0"/>
+        <c:smooth val="0"/>
         <c:axId val="91754508"/>
         <c:axId val="37814408"/>
       </c:lineChart>
@@ -2138,7 +2289,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -2147,7 +2298,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -2174,7 +2325,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
+              <a:srgbClr val="D9D9D9"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -2184,7 +2335,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -2192,6 +2343,7 @@
                 <a:ea typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="37814408"/>
@@ -2212,7 +2364,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2222,7 +2374,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="f2f2f2"/>
+                <a:srgbClr val="F2F2F2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2235,7 +2387,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -2244,7 +2396,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -2278,7 +2430,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -2286,6 +2438,7 @@
                 <a:ea typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="91754508"/>
@@ -2313,7 +2466,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+            <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
               <a:solidFill>
                 <a:srgbClr val="595959"/>
               </a:solidFill>
@@ -2321,28 +2474,35 @@
               <a:ea typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln w="9360">
       <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
+        <a:srgbClr val="D9D9D9"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -2356,14 +2516,20 @@
       <xdr:row>27</xdr:row>
       <xdr:rowOff>14040</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Γράφημα 1"/>
+        <xdr:cNvPr id="2" name="Γράφημα 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="38160" y="1245960"/>
-        <a:ext cx="9866880" cy="3806640"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2386,14 +2552,20 @@
       <xdr:row>57</xdr:row>
       <xdr:rowOff>113040</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name="Γράφημα 3"/>
+        <xdr:cNvPr id="3" name="Γράφημα 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="6883200"/>
-        <a:ext cx="9963360" cy="3850200"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2416,14 +2588,20 @@
       <xdr:row>58</xdr:row>
       <xdr:rowOff>24120</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 4"/>
+        <xdr:cNvPr id="4" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11923920" y="6721200"/>
-        <a:ext cx="11656080" cy="4104360"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2446,14 +2624,20 @@
       <xdr:row>26</xdr:row>
       <xdr:rowOff>138600</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 5"/>
+        <xdr:cNvPr id="5" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11905200" y="1327320"/>
-        <a:ext cx="11145600" cy="3669120"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2478,11 +2662,17 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Image 1" descr=""/>
+        <xdr:cNvPr id="6" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -2504,121 +2694,127 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:E6" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A2:E6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Πίνακας1" displayName="Πίνακας1" ref="A2:E6" totalsRowShown="0">
+  <autoFilter ref="A2:E6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Ν"/>
-    <tableColumn id="2" name="Μ"/>
-    <tableColumn id="3" name="unoptimised (s)"/>
-    <tableColumn id="4" name="optimised (s)"/>
-    <tableColumn id="5" name="Optimisation"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Ν"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Μ"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="unoptimised (s)"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="optimised (s)"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Optimisation"/>
   </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Πίνακας13" displayName="Πίνακας13" ref="I2:M6" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="I2:M6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Πίνακας13" displayName="Πίνακας13" ref="I2:M6" totalsRowShown="0">
+  <autoFilter ref="I2:M6" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Ν"/>
-    <tableColumn id="2" name="Μ"/>
-    <tableColumn id="3" name="unoptimised (s)"/>
-    <tableColumn id="4" name="optimised (s)"/>
-    <tableColumn id="5" name="Optimisation"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Ν"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Μ"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="unoptimised (s)"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="optimised (s)"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Optimisation"/>
   </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Πίνακας14" displayName="Πίνακας14" ref="A31:E35" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A31:E35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Πίνακας14" displayName="Πίνακας14" ref="A31:E35" totalsRowShown="0">
+  <autoFilter ref="A31:E35" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Ν"/>
-    <tableColumn id="2" name="Μ"/>
-    <tableColumn id="3" name="ARM"/>
-    <tableColumn id="4" name="x86"/>
-    <tableColumn id="5" name="Optimisation"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Ν"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Μ"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="ARM"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="x86" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Optimisation"/>
   </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Πίνακας145" displayName="Πίνακας145" ref="I31:M35" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="I31:M35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Πίνακας145" displayName="Πίνακας145" ref="I31:M35" totalsRowShown="0">
+  <autoFilter ref="I31:M35" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Ν"/>
-    <tableColumn id="2" name="Μ"/>
-    <tableColumn id="3" name="ARM"/>
-    <tableColumn id="4" name="x86"/>
-    <tableColumn id="5" name="Optimisation"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Ν"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Μ"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="ARM"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="x86" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Optimisation"/>
   </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Πίνακας16" displayName="Πίνακας16" ref="Q2:U7" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="Q2:U7"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Ν"/>
-    <tableColumn id="2" name="Μ"/>
-    <tableColumn id="3" name="unoptimised (s)"/>
-    <tableColumn id="4" name="optimised (s)"/>
-    <tableColumn id="5" name="Optimisation"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Πίνακας16" displayName="Πίνακας16" ref="Q2:V7" totalsRowShown="0">
+  <autoFilter ref="Q2:V7" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Ν"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Μ"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="unoptimised (s)"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="sol 1"/>
+    <tableColumn id="7" xr3:uid="{70D81907-0F82-4F10-B2C0-AB1DC0D82CD5}" name="sol 2" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Optimisation"/>
   </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0e2841"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="e8e8e8"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="e97132"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196b24"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0f9ed5"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="a02b93"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4ea72e"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607d"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" pitchFamily="0" charset="1"/>
-        <a:ea typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:cs typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Aptos Display"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" pitchFamily="0" charset="1"/>
-        <a:ea typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:cs typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Aptos Narrow"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -2648,7 +2844,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -2672,7 +2868,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -2732,514 +2928,519 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:U35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T5" activeCellId="0" sqref="T5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="30.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="28.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="26.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="25.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="29.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="44.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="16.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="20.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="22.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="27.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="26.12"/>
+    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.21875" customWidth="1"/>
+    <col min="4" max="4" width="30.21875" customWidth="1"/>
+    <col min="5" max="5" width="28.88671875" customWidth="1"/>
+    <col min="9" max="9" width="26.77734375" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" customWidth="1"/>
+    <col min="11" max="11" width="29.21875" customWidth="1"/>
+    <col min="12" max="12" width="23" customWidth="1"/>
+    <col min="13" max="13" width="44.6640625" customWidth="1"/>
+    <col min="17" max="17" width="16.88671875" customWidth="1"/>
+    <col min="18" max="18" width="20.6640625" customWidth="1"/>
+    <col min="19" max="19" width="22.77734375" customWidth="1"/>
+    <col min="20" max="21" width="27.44140625" customWidth="1"/>
+    <col min="22" max="22" width="26.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:22" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="Q1" s="2" t="s">
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="Q1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="T2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="U2" s="3" t="s">
+      <c r="T2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="V2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="n">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>32</v>
       </c>
-      <c r="B3" s="4" t="n">
+      <c r="B3" s="2">
         <v>32</v>
       </c>
-      <c r="C3" s="4" t="n">
-        <v>1.3E-005</v>
-      </c>
-      <c r="D3" s="4" t="n">
-        <v>1.2E-005</v>
-      </c>
-      <c r="E3" s="5" t="n">
-        <f aca="false">(C3-D3)/C3</f>
-        <v>0.0769230769230768</v>
-      </c>
-      <c r="I3" s="4" t="n">
+      <c r="C3" s="2">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.5E-5</v>
+      </c>
+      <c r="E3" s="3">
+        <f>(C3-D3)/C3</f>
+        <v>0.25000000000000006</v>
+      </c>
+      <c r="I3" s="2">
         <v>32</v>
       </c>
-      <c r="J3" s="4" t="n">
+      <c r="J3" s="2">
         <v>32</v>
       </c>
-      <c r="K3" s="4" t="n">
-        <v>9.8E-005</v>
-      </c>
-      <c r="L3" s="4" t="n">
-        <v>4.5E-005</v>
-      </c>
-      <c r="M3" s="5" t="n">
-        <f aca="false">(K3-L3)/K3</f>
-        <v>0.540816326530612</v>
-      </c>
-      <c r="Q3" s="4" t="n">
+      <c r="K3" s="2">
+        <v>9.7999999999999997E-5</v>
+      </c>
+      <c r="L3" s="2">
+        <v>4.5000000000000003E-5</v>
+      </c>
+      <c r="M3" s="3">
+        <f>(K3-L3)/K3</f>
+        <v>0.54081632653061218</v>
+      </c>
+      <c r="Q3" s="2">
         <v>32</v>
       </c>
-      <c r="R3" s="4" t="n">
+      <c r="R3" s="2">
         <v>32</v>
       </c>
-      <c r="S3" s="4" t="n">
-        <v>0.002565564</v>
-      </c>
-      <c r="T3" s="4" t="n">
-        <v>0.000817334</v>
-      </c>
-      <c r="U3" s="5" t="n">
-        <f aca="false">(S3-T3)/S3</f>
-        <v>0.681421317106102</v>
+      <c r="S3" s="2">
+        <v>2.5655640000000002E-3</v>
+      </c>
+      <c r="T3" s="2">
+        <v>8.1733399999999996E-4</v>
+      </c>
+      <c r="U3" s="2"/>
+      <c r="V3" s="3">
+        <f>(S3-T3)/S3</f>
+        <v>0.68142131710610232</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="n">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
         <v>32</v>
       </c>
-      <c r="B4" s="4" t="n">
+      <c r="B4" s="2">
         <v>65536</v>
       </c>
-      <c r="C4" s="4" t="n">
-        <v>0.034103</v>
-      </c>
-      <c r="D4" s="4" t="n">
-        <v>0.018605</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <f aca="false">(C4-D4)/C4</f>
-        <v>0.454446822860159</v>
-      </c>
-      <c r="I4" s="4" t="n">
+      <c r="C4" s="2">
+        <v>3.7108000000000002E-2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2.4056999999999999E-2</v>
+      </c>
+      <c r="E4" s="3">
+        <f>(C4-D4)/C4</f>
+        <v>0.35170313678991061</v>
+      </c>
+      <c r="I4" s="2">
         <v>32</v>
       </c>
-      <c r="J4" s="4" t="n">
+      <c r="J4" s="2">
         <v>65536</v>
       </c>
-      <c r="K4" s="4" t="n">
+      <c r="K4" s="2">
         <v>0.175177</v>
       </c>
-      <c r="L4" s="4" t="n">
-        <v>0.076079</v>
-      </c>
-      <c r="M4" s="5" t="n">
-        <f aca="false">(K4-L4)/K4</f>
-        <v>0.565702118428789</v>
-      </c>
-      <c r="Q4" s="4" t="n">
+      <c r="L4" s="2">
+        <v>7.6078999999999994E-2</v>
+      </c>
+      <c r="M4" s="3">
+        <f>(K4-L4)/K4</f>
+        <v>0.56570211842878915</v>
+      </c>
+      <c r="Q4" s="2">
         <v>32</v>
       </c>
-      <c r="R4" s="4" t="n">
+      <c r="R4" s="2">
         <v>65536</v>
       </c>
-      <c r="S4" s="4" t="n">
-        <v>3.268688927</v>
-      </c>
-      <c r="T4" s="4" t="n">
-        <v>0.380162242</v>
-      </c>
-      <c r="U4" s="5" t="n">
-        <f aca="false">(S4-T4)/S4</f>
-        <v>0.883695802662717</v>
+      <c r="S4" s="2">
+        <v>3.2686889269999999</v>
+      </c>
+      <c r="T4" s="2">
+        <v>0.38016224199999998</v>
+      </c>
+      <c r="U4" s="2"/>
+      <c r="V4" s="3">
+        <f>(S4-T4)/S4</f>
+        <v>0.88369580266271697</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="n">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>256</v>
       </c>
-      <c r="B5" s="4" t="n">
+      <c r="B5" s="2">
         <v>65536</v>
       </c>
-      <c r="C5" s="4" t="n">
-        <v>0.263528</v>
-      </c>
-      <c r="D5" s="4" t="n">
-        <v>0.137813</v>
-      </c>
-      <c r="E5" s="5" t="n">
-        <f aca="false">(C5-D5)/C5</f>
-        <v>0.477046082389727</v>
-      </c>
-      <c r="I5" s="4" t="n">
+      <c r="C5" s="2">
+        <v>0.30333500000000002</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.19692599999999999</v>
+      </c>
+      <c r="E5" s="3">
+        <f>(C5-D5)/C5</f>
+        <v>0.35079697364300205</v>
+      </c>
+      <c r="I5" s="2">
         <v>256</v>
       </c>
-      <c r="J5" s="4" t="n">
+      <c r="J5" s="2">
         <v>65536</v>
       </c>
-      <c r="K5" s="4" t="n">
-        <v>1.402216</v>
-      </c>
-      <c r="L5" s="4" t="n">
-        <v>0.586488</v>
-      </c>
-      <c r="M5" s="5" t="n">
-        <f aca="false">(K5-L5)/K5</f>
-        <v>0.581742042595435</v>
-      </c>
-      <c r="Q5" s="4" t="n">
+      <c r="K5" s="2">
+        <v>1.4022159999999999</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0.58648800000000001</v>
+      </c>
+      <c r="M5" s="3">
+        <f>(K5-L5)/K5</f>
+        <v>0.58174204259543461</v>
+      </c>
+      <c r="Q5" s="2">
         <v>256</v>
       </c>
-      <c r="R5" s="4" t="n">
+      <c r="R5" s="2">
         <v>65536</v>
       </c>
-      <c r="S5" s="4" t="n">
-        <v>0.443408594</v>
-      </c>
-      <c r="T5" s="4" t="n">
-        <v>2.176</v>
-      </c>
-      <c r="U5" s="5" t="n">
-        <f aca="false">(S5-T5)/S5</f>
-        <v>-3.90743758565943</v>
+      <c r="S5" s="2">
+        <v>0.44340859399999999</v>
+      </c>
+      <c r="T5" s="2">
+        <v>2.1760000000000002</v>
+      </c>
+      <c r="U5" s="2"/>
+      <c r="V5" s="3">
+        <f>(S5-T5)/S5</f>
+        <v>-3.9074375856594248</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="n">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
         <v>256</v>
       </c>
-      <c r="B6" s="4" t="n">
+      <c r="B6" s="2">
         <v>300000</v>
       </c>
-      <c r="C6" s="6" t="n">
-        <v>1.196854</v>
-      </c>
-      <c r="D6" s="4" t="n">
-        <v>0.628575</v>
-      </c>
-      <c r="E6" s="5" t="n">
-        <f aca="false">(C6-D6)/C6</f>
-        <v>0.474810628531133</v>
-      </c>
-      <c r="I6" s="4" t="n">
+      <c r="C6" s="4">
+        <v>1.3882559999999999</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.89723900000000001</v>
+      </c>
+      <c r="E6" s="3">
+        <f>(C6-D6)/C6</f>
+        <v>0.35369341101353063</v>
+      </c>
+      <c r="I6" s="2">
         <v>256</v>
       </c>
-      <c r="J6" s="4" t="n">
+      <c r="J6" s="2">
         <v>300000</v>
       </c>
-      <c r="K6" s="6" t="n">
-        <v>6.417753</v>
-      </c>
-      <c r="L6" s="4" t="n">
-        <v>2.685104</v>
-      </c>
-      <c r="M6" s="5" t="n">
-        <f aca="false">(K6-L6)/K6</f>
-        <v>0.581613066130778</v>
-      </c>
-      <c r="Q6" s="4" t="n">
+      <c r="K6" s="4">
+        <v>6.4177530000000003</v>
+      </c>
+      <c r="L6" s="2">
+        <v>2.6851039999999999</v>
+      </c>
+      <c r="M6" s="3">
+        <f>(K6-L6)/K6</f>
+        <v>0.58161306613077823</v>
+      </c>
+      <c r="Q6" s="2">
         <v>256</v>
       </c>
-      <c r="R6" s="4" t="n">
+      <c r="R6" s="2">
         <v>300000</v>
       </c>
-      <c r="S6" s="7" t="s">
+      <c r="S6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="T6" s="8" t="s">
+      <c r="T6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="U6" s="9" t="s">
+      <c r="U6" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="V6" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="30" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="s">
+    <row r="30" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="I30" s="2" t="s">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="I30" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
     </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I31" s="3" t="s">
+      <c r="I31" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J31" s="3" t="s">
+      <c r="J31" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K31" s="3" t="s">
+      <c r="K31" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L31" s="3" t="s">
+      <c r="L31" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="M31" s="3" t="s">
+      <c r="M31" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="n">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
         <v>32</v>
       </c>
-      <c r="B32" s="4" t="n">
+      <c r="B32" s="2">
         <v>32</v>
       </c>
-      <c r="C32" s="4" t="n">
-        <v>4.5E-005</v>
-      </c>
-      <c r="D32" s="4" t="n">
-        <v>1.2E-005</v>
-      </c>
-      <c r="E32" s="5" t="n">
-        <f aca="false">(C32-D32)/C32</f>
-        <v>0.733333333333333</v>
-      </c>
-      <c r="I32" s="4" t="n">
+      <c r="C32" s="2">
+        <v>4.5000000000000003E-5</v>
+      </c>
+      <c r="D32" s="2">
+        <v>1.5E-5</v>
+      </c>
+      <c r="E32" s="3">
+        <f>(C32-D32)/C32</f>
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="I32" s="2">
         <v>32</v>
       </c>
-      <c r="J32" s="4" t="n">
+      <c r="J32" s="2">
         <v>32</v>
       </c>
-      <c r="K32" s="4" t="n">
-        <v>9.8E-005</v>
-      </c>
-      <c r="L32" s="4" t="n">
-        <v>1.3E-005</v>
-      </c>
-      <c r="M32" s="5" t="n">
-        <f aca="false">(K32-L32)/K32</f>
-        <v>0.86734693877551</v>
+      <c r="K32" s="2">
+        <v>9.7999999999999997E-5</v>
+      </c>
+      <c r="L32" s="2">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="M32" s="3">
+        <f>(K32-L32)/K32</f>
+        <v>0.79591836734693877</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="4" t="n">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
         <v>32</v>
       </c>
-      <c r="B33" s="4" t="n">
+      <c r="B33" s="2">
         <v>65536</v>
       </c>
-      <c r="C33" s="4" t="n">
-        <v>0.076079</v>
-      </c>
-      <c r="D33" s="4" t="n">
-        <v>0.018605</v>
-      </c>
-      <c r="E33" s="5" t="n">
-        <f aca="false">(C33-D33)/C33</f>
-        <v>0.755451570078471</v>
-      </c>
-      <c r="I33" s="4" t="n">
+      <c r="C33" s="2">
+        <v>7.6078999999999994E-2</v>
+      </c>
+      <c r="D33" s="2">
+        <v>2.4056999999999999E-2</v>
+      </c>
+      <c r="E33" s="3">
+        <f>(C33-D33)/C33</f>
+        <v>0.6837892191011975</v>
+      </c>
+      <c r="I33" s="2">
         <v>32</v>
       </c>
-      <c r="J33" s="4" t="n">
+      <c r="J33" s="2">
         <v>65536</v>
       </c>
-      <c r="K33" s="4" t="n">
+      <c r="K33" s="2">
         <v>0.175177</v>
       </c>
-      <c r="L33" s="4" t="n">
-        <v>0.034103</v>
-      </c>
-      <c r="M33" s="5" t="n">
-        <f aca="false">(K33-L33)/K33</f>
-        <v>0.805322616553543</v>
+      <c r="L33" s="2">
+        <v>3.7108000000000002E-2</v>
+      </c>
+      <c r="M33" s="3">
+        <f>(K33-L33)/K33</f>
+        <v>0.78816853810717158</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="4" t="n">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
         <v>256</v>
       </c>
-      <c r="B34" s="4" t="n">
+      <c r="B34" s="2">
         <v>65536</v>
       </c>
-      <c r="C34" s="4" t="n">
-        <v>0.586488</v>
-      </c>
-      <c r="D34" s="4" t="n">
-        <v>0.137813</v>
-      </c>
-      <c r="E34" s="5" t="n">
-        <f aca="false">(C34-D34)/C34</f>
-        <v>0.765019915155979</v>
-      </c>
-      <c r="I34" s="4" t="n">
+      <c r="C34" s="2">
+        <v>0.58648800000000001</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.19692599999999999</v>
+      </c>
+      <c r="E34" s="3">
+        <f>(C34-D34)/C34</f>
+        <v>0.66422842411097927</v>
+      </c>
+      <c r="I34" s="2">
         <v>256</v>
       </c>
-      <c r="J34" s="4" t="n">
+      <c r="J34" s="2">
         <v>65536</v>
       </c>
-      <c r="K34" s="4" t="n">
-        <v>1.402216</v>
-      </c>
-      <c r="L34" s="4" t="n">
-        <v>0.263528</v>
-      </c>
-      <c r="M34" s="5" t="n">
-        <f aca="false">(K34-L34)/K34</f>
-        <v>0.812063191405604</v>
+      <c r="K34" s="2">
+        <v>1.4022159999999999</v>
+      </c>
+      <c r="L34" s="2">
+        <v>0.30333500000000002</v>
+      </c>
+      <c r="M34" s="3">
+        <f>(K34-L34)/K34</f>
+        <v>0.78367455513273276</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="4" t="n">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
         <v>256</v>
       </c>
-      <c r="B35" s="4" t="n">
+      <c r="B35" s="2">
         <v>300000</v>
       </c>
-      <c r="C35" s="4" t="n">
-        <v>2.685104</v>
-      </c>
-      <c r="D35" s="4" t="n">
-        <v>0.628575</v>
-      </c>
-      <c r="E35" s="5" t="n">
-        <f aca="false">(C35-D35)/C35</f>
-        <v>0.765902922195937</v>
-      </c>
-      <c r="I35" s="4" t="n">
+      <c r="C35" s="2">
+        <v>2.6851039999999999</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.89723900000000001</v>
+      </c>
+      <c r="E35" s="3">
+        <f>(C35-D35)/C35</f>
+        <v>0.66584571770776857</v>
+      </c>
+      <c r="I35" s="2">
         <v>256</v>
       </c>
-      <c r="J35" s="4" t="n">
+      <c r="J35" s="2">
         <v>300000</v>
       </c>
-      <c r="K35" s="6" t="n">
-        <v>6.417753</v>
-      </c>
-      <c r="L35" s="6" t="n">
-        <v>1.196854</v>
-      </c>
-      <c r="M35" s="5" t="n">
-        <f aca="false">(K35-L35)/K35</f>
-        <v>0.813508871407173</v>
+      <c r="K35" s="4">
+        <v>6.4177530000000003</v>
+      </c>
+      <c r="L35" s="4">
+        <v>1.3882559999999999</v>
+      </c>
+      <c r="M35" s="3">
+        <f>(K35-L35)/K35</f>
+        <v>0.78368503742665074</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="I1:M1"/>
-    <mergeCell ref="Q1:U1"/>
+    <mergeCell ref="Q1:V1"/>
     <mergeCell ref="A30:E30"/>
     <mergeCell ref="I30:M30"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <drawing r:id="rId1"/>
-  <tableParts>
+  <tableParts count="5">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>

</xml_diff>

<commit_message>
added new table fpga vs x86 in report_spithas
</commit_message>
<xml_diff>
--- a/lab3/lsal/lab3 LSAL imlementation.xlsx
+++ b/lab3/lsal/lab3 LSAL imlementation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sstat\Documents\GitHub\Embedded-Systems\lab3\lsal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13449057-7542-4342-87B0-4497DD571751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36105AEC-5EAF-4546-8A90-117066F88837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="8880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Φύλλο1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="15">
   <si>
     <t>x86</t>
   </si>
@@ -76,6 +76,12 @@
   <si>
     <t>sol 2</t>
   </si>
+  <si>
+    <t>FPGA x86</t>
+  </si>
+  <si>
+    <t>FPGA best solution</t>
+  </si>
 </sst>
 </file>
 
@@ -105,7 +111,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -118,8 +124,14 @@
         <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -142,15 +154,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -163,6 +181,13 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2728,7 +2753,7 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Ν"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Μ"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="ARM"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="x86" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="x86" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Optimisation"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2742,7 +2767,7 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Ν"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Μ"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="ARM"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="x86" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="x86" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Optimisation"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2942,8 +2967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2966,475 +2991,562 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="I1" s="1" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="I1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="Q1" s="1" t="s">
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="Q1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="S2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="T2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="U2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="V2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>32</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>32</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>1.5E-5</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <f>(C3-D3)/C3</f>
         <v>0.25000000000000006</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <v>32</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="1">
         <v>32</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="1">
         <v>9.7999999999999997E-5</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="1">
         <v>4.5000000000000003E-5</v>
       </c>
-      <c r="M3" s="3">
+      <c r="M3" s="2">
         <f>(K3-L3)/K3</f>
         <v>0.54081632653061218</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="Q3" s="1">
         <v>32</v>
       </c>
-      <c r="R3" s="2">
+      <c r="R3" s="1">
         <v>32</v>
       </c>
-      <c r="S3" s="2">
+      <c r="S3" s="1">
         <v>2.5655640000000002E-3</v>
       </c>
-      <c r="T3" s="2">
+      <c r="T3" s="1">
         <v>8.1733399999999996E-4</v>
       </c>
-      <c r="U3" s="2"/>
-      <c r="V3" s="3">
+      <c r="U3" s="1"/>
+      <c r="V3" s="2">
         <f>(S3-T3)/S3</f>
         <v>0.68142131710610232</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>32</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>65536</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>3.7108000000000002E-2</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>2.4056999999999999E-2</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <f>(C4-D4)/C4</f>
         <v>0.35170313678991061</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <v>32</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
         <v>65536</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="1">
         <v>0.175177</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="1">
         <v>7.6078999999999994E-2</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M4" s="2">
         <f>(K4-L4)/K4</f>
         <v>0.56570211842878915</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="Q4" s="1">
         <v>32</v>
       </c>
-      <c r="R4" s="2">
+      <c r="R4" s="1">
         <v>65536</v>
       </c>
-      <c r="S4" s="2">
+      <c r="S4" s="1">
         <v>3.2686889269999999</v>
       </c>
-      <c r="T4" s="2">
+      <c r="T4" s="1">
         <v>0.38016224199999998</v>
       </c>
-      <c r="U4" s="2"/>
-      <c r="V4" s="3">
+      <c r="U4" s="1"/>
+      <c r="V4" s="2">
         <f>(S4-T4)/S4</f>
         <v>0.88369580266271697</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>256</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>65536</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>0.30333500000000002</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>0.19692599999999999</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <f>(C5-D5)/C5</f>
         <v>0.35079697364300205</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <v>256</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1">
         <v>65536</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="1">
         <v>1.4022159999999999</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="1">
         <v>0.58648800000000001</v>
       </c>
-      <c r="M5" s="3">
+      <c r="M5" s="2">
         <f>(K5-L5)/K5</f>
         <v>0.58174204259543461</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="Q5" s="1">
         <v>256</v>
       </c>
-      <c r="R5" s="2">
+      <c r="R5" s="1">
         <v>65536</v>
       </c>
-      <c r="S5" s="2">
+      <c r="S5" s="1">
         <v>0.44340859399999999</v>
       </c>
-      <c r="T5" s="2">
+      <c r="T5" s="1">
         <v>2.1760000000000002</v>
       </c>
-      <c r="U5" s="2"/>
-      <c r="V5" s="3">
+      <c r="U5" s="1"/>
+      <c r="V5" s="2">
         <f>(S5-T5)/S5</f>
         <v>-3.9074375856594248</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>256</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>300000</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>1.3882559999999999</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>0.89723900000000001</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <f>(C6-D6)/C6</f>
         <v>0.35369341101353063</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="1">
         <v>256</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="1">
         <v>300000</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="3">
         <v>6.4177530000000003</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="1">
         <v>2.6851039999999999</v>
       </c>
-      <c r="M6" s="3">
+      <c r="M6" s="2">
         <f>(K6-L6)/K6</f>
         <v>0.58161306613077823</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="Q6" s="1">
         <v>256</v>
       </c>
-      <c r="R6" s="2">
+      <c r="R6" s="1">
         <v>300000</v>
       </c>
-      <c r="S6" s="5" t="s">
+      <c r="S6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="T6" s="6" t="s">
+      <c r="T6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="U6" s="6" t="s">
+      <c r="U6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="V6" s="7" t="s">
+      <c r="V6" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:22" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="I30" s="1" t="s">
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="I30" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="Q30" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="R30" s="8"/>
+      <c r="S30" s="8"/>
+      <c r="T30" s="8"/>
+      <c r="U30" s="8"/>
+      <c r="V30" s="9"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="I31" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J31" s="2" t="s">
+      <c r="J31" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K31" s="2" t="s">
+      <c r="K31" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L31" s="2" t="s">
+      <c r="L31" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M31" s="2" t="s">
+      <c r="M31" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="Q31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="U31" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="2">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
         <v>32</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="1">
         <v>32</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="1">
         <v>4.5000000000000003E-5</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="1">
         <v>1.5E-5</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="2">
         <f>(C32-D32)/C32</f>
         <v>0.66666666666666674</v>
       </c>
-      <c r="I32" s="2">
+      <c r="I32" s="1">
         <v>32</v>
       </c>
-      <c r="J32" s="2">
+      <c r="J32" s="1">
         <v>32</v>
       </c>
-      <c r="K32" s="2">
+      <c r="K32" s="1">
         <v>9.7999999999999997E-5</v>
       </c>
-      <c r="L32" s="2">
+      <c r="L32" s="1">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="M32" s="3">
+      <c r="M32" s="2">
         <f>(K32-L32)/K32</f>
         <v>0.79591836734693877</v>
       </c>
+      <c r="Q32" s="1">
+        <v>32</v>
+      </c>
+      <c r="R32" s="1">
+        <v>32</v>
+      </c>
+      <c r="S32" s="1">
+        <v>1.5E-5</v>
+      </c>
+      <c r="T32" s="1">
+        <v>8.1733399999999996E-4</v>
+      </c>
+      <c r="U32" s="2">
+        <f>(S32-T32)/S32</f>
+        <v>-53.488933333333328</v>
+      </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
         <v>32</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="1">
         <v>65536</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="1">
         <v>7.6078999999999994E-2</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="1">
         <v>2.4056999999999999E-2</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33" s="2">
         <f>(C33-D33)/C33</f>
         <v>0.6837892191011975</v>
       </c>
-      <c r="I33" s="2">
+      <c r="I33" s="1">
         <v>32</v>
       </c>
-      <c r="J33" s="2">
+      <c r="J33" s="1">
         <v>65536</v>
       </c>
-      <c r="K33" s="2">
+      <c r="K33" s="1">
         <v>0.175177</v>
       </c>
-      <c r="L33" s="2">
+      <c r="L33" s="1">
         <v>3.7108000000000002E-2</v>
       </c>
-      <c r="M33" s="3">
+      <c r="M33" s="2">
         <f>(K33-L33)/K33</f>
         <v>0.78816853810717158</v>
       </c>
+      <c r="Q33" s="1">
+        <v>32</v>
+      </c>
+      <c r="R33" s="1">
+        <v>65536</v>
+      </c>
+      <c r="S33" s="1">
+        <v>2.4056999999999999E-2</v>
+      </c>
+      <c r="T33" s="1">
+        <v>0.38016224199999998</v>
+      </c>
+      <c r="U33" s="2">
+        <f t="shared" ref="U33:U34" si="0">(S33-T33)/S33</f>
+        <v>-14.802562331130233</v>
+      </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
         <v>256</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="1">
         <v>65536</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="1">
         <v>0.58648800000000001</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="1">
         <v>0.19692599999999999</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="2">
         <f>(C34-D34)/C34</f>
         <v>0.66422842411097927</v>
       </c>
-      <c r="I34" s="2">
+      <c r="I34" s="1">
         <v>256</v>
       </c>
-      <c r="J34" s="2">
+      <c r="J34" s="1">
         <v>65536</v>
       </c>
-      <c r="K34" s="2">
+      <c r="K34" s="1">
         <v>1.4022159999999999</v>
       </c>
-      <c r="L34" s="2">
+      <c r="L34" s="1">
         <v>0.30333500000000002</v>
       </c>
-      <c r="M34" s="3">
+      <c r="M34" s="2">
         <f>(K34-L34)/K34</f>
         <v>0.78367455513273276</v>
       </c>
+      <c r="Q34" s="1">
+        <v>256</v>
+      </c>
+      <c r="R34" s="1">
+        <v>65536</v>
+      </c>
+      <c r="S34" s="1">
+        <v>0.19692599999999999</v>
+      </c>
+      <c r="T34" s="1">
+        <v>2.1760000000000002</v>
+      </c>
+      <c r="U34" s="2">
+        <f t="shared" si="0"/>
+        <v>-10.049835978997189</v>
+      </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A35" s="2">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
         <v>256</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35" s="1">
         <v>300000</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="1">
         <v>2.6851039999999999</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="1">
         <v>0.89723900000000001</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35" s="2">
         <f>(C35-D35)/C35</f>
         <v>0.66584571770776857</v>
       </c>
-      <c r="I35" s="2">
+      <c r="I35" s="1">
         <v>256</v>
       </c>
-      <c r="J35" s="2">
+      <c r="J35" s="1">
         <v>300000</v>
       </c>
-      <c r="K35" s="4">
+      <c r="K35" s="3">
         <v>6.4177530000000003</v>
       </c>
-      <c r="L35" s="4">
+      <c r="L35" s="3">
         <v>1.3882559999999999</v>
       </c>
-      <c r="M35" s="3">
+      <c r="M35" s="2">
         <f>(K35-L35)/K35</f>
         <v>0.78368503742665074</v>
       </c>
+      <c r="Q35" s="1">
+        <v>256</v>
+      </c>
+      <c r="R35" s="1">
+        <v>300000</v>
+      </c>
+      <c r="S35" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="T35" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="U35" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="I1:M1"/>
     <mergeCell ref="Q1:V1"/>
     <mergeCell ref="A30:E30"/>
     <mergeCell ref="I30:M30"/>
+    <mergeCell ref="Q30:U30"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
final reports without sol3
</commit_message>
<xml_diff>
--- a/lab3/lsal/lab3 LSAL imlementation.xlsx
+++ b/lab3/lsal/lab3 LSAL imlementation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sstat\Documents\GitHub\Embedded-Systems\lab3\lsal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE7B776-C018-4C9A-84CF-EC5FDD0A61AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F636DA-00F9-4AA7-8D0F-81CEAB7D5DA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="17">
   <si>
     <t>x86</t>
   </si>
@@ -86,16 +86,7 @@
     <t>sol 3</t>
   </si>
   <si>
-    <t>pipeline=32</t>
-  </si>
-  <si>
-    <t>no pipeline</t>
-  </si>
-  <si>
-    <t>buffers</t>
-  </si>
-  <si>
-    <t>read after write dependencies</t>
+    <t>(x86 is fatser)</t>
   </si>
 </sst>
 </file>
@@ -106,7 +97,7 @@
     <numFmt numFmtId="164" formatCode="0.0000%"/>
     <numFmt numFmtId="165" formatCode="#,##0.000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -124,6 +115,12 @@
       <sz val="8"/>
       <name val="Aptos Narrow"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -146,7 +143,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -191,11 +188,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -210,19 +216,34 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2581,6 +2602,1043 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="2000" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Aptos Display"/>
+                <a:ea typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Chart Title</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.43021866218791399"/>
+          <c:y val="2.8156578043755501E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="38160" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="156082"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr wrap="square"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Φύλλο1!$Q$3:$Q$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-50F7-4DC0-B48F-FA3220C5C93D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="38160" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="E97132"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr wrap="square"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Φύλλο1!$R$3:$R$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-50F7-4DC0-B48F-FA3220C5C93D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Φύλλο1!$S$2:$S$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5655640000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2686889269999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.5359965000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-B4A4-4883-9877-92E205634A12}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Φύλλο1!$T$2:$T$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.1733399999999996E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.38016224199999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1760000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-B4A4-4883-9877-92E205634A12}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:smooth val="0"/>
+        <c:axId val="91754508"/>
+        <c:axId val="37814408"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="91754508"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Title</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="D9D9D9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Aptos Narrow"/>
+                <a:ea typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="37814408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="37814408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="D9D9D9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="F2F2F2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Title</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="12600">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Aptos Narrow"/>
+                <a:ea typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="91754508"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:solidFill>
+                <a:srgbClr val="595959"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow"/>
+              <a:ea typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="D9D9D9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="2000" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Aptos Display"/>
+                <a:ea typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Chart Title</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.43021866218791399"/>
+          <c:y val="2.8156578043755501E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Φύλλο1!$Q$32:$R$32</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38160" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="156082"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr wrap="square"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Φύλλο1!$Q$32:$S$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-50F7-4DC0-B48F-FA3220C5C93D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Φύλλο1!$Q$33:$R$33</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65536</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38160" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="E97132"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr wrap="square"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Φύλλο1!$Q$33:$S$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4056999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-50F7-4DC0-B48F-FA3220C5C93D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Φύλλο1!$Q$34:$R$34</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65536</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Φύλλο1!$Q$34:$S$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19692599999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-C049-4AE9-8702-9D140AD03769}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:smooth val="0"/>
+        <c:axId val="91754508"/>
+        <c:axId val="37814408"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="91754508"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Title</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="D9D9D9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Aptos Narrow"/>
+                <a:ea typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="37814408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="37814408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="D9D9D9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="F2F2F2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Aptos Narrow"/>
+                    <a:ea typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Title</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="12600">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Aptos Narrow"/>
+                <a:ea typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="91754508"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:solidFill>
+                <a:srgbClr val="595959"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow"/>
+              <a:ea typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="D9D9D9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -2768,6 +3826,78 @@
         </a:ln>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>302712</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>84550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>1753644</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>9394</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A70F64C3-F918-0382-99C0-89B48440E0C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>292274</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>168058</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>1826712</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>20877</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30EEFA64-3709-3F8A-2EED-278BA7C7D841}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3019,12 +4149,352 @@
 </a:theme>
 </file>
 
+<file path=xl/theme/themeOverride1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:srgbClr val="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:srgbClr val="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="0E2841"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E8E8E8"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="156082"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="E97132"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="196B24"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="0F9ED5"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="A02B93"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="4EA72E"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="467886"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="96607D"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Aptos Display"/>
+      <a:ea typeface="Arial"/>
+      <a:cs typeface="Arial"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Aptos Narrow"/>
+      <a:ea typeface="Arial"/>
+      <a:cs typeface="Arial"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme>
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+        <a:tileRect/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+        <a:tileRect/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
+<file path=xl/theme/themeOverride2.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:srgbClr val="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:srgbClr val="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="0E2841"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E8E8E8"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="156082"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="E97132"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="196B24"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="0F9ED5"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="A02B93"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="4EA72E"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="467886"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="96607D"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Aptos Display"/>
+      <a:ea typeface="Arial"/>
+      <a:cs typeface="Arial"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Aptos Narrow"/>
+      <a:ea typeface="Arial"/>
+      <a:cs typeface="Arial"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme>
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+        <a:tileRect/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+        <a:tileRect/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y19" sqref="Y19"/>
+    <sheetView tabSelected="1" topLeftCell="M30" zoomScale="93" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V37" sqref="V37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3047,29 +4517,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="I1" s="8" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="I1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="Q1" s="8" t="s">
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="Q1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -3169,8 +4639,12 @@
       <c r="T3" s="1">
         <v>8.1733399999999996E-4</v>
       </c>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
+      <c r="U3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="W3" s="2">
         <f>(S3-T3)/S3</f>
         <v>0.68142131710610232</v>
@@ -3224,7 +4698,7 @@
       <c r="U4" s="1">
         <v>0.17579239999999999</v>
       </c>
-      <c r="V4" s="1"/>
+      <c r="V4" s="5"/>
       <c r="W4" s="2">
         <f>(S4-U4)/S4</f>
         <v>0.94621929344578459</v>
@@ -3263,23 +4737,27 @@
         <f>(K5-L5)/K5</f>
         <v>0.58174204259543461</v>
       </c>
-      <c r="Q5" s="1">
+      <c r="Q5" s="8">
         <v>256</v>
       </c>
-      <c r="R5" s="1">
+      <c r="R5" s="8">
         <v>65536</v>
       </c>
-      <c r="S5" s="1">
-        <v>0.44340859399999999</v>
-      </c>
-      <c r="T5" s="1">
+      <c r="S5" s="8">
+        <v>5.5359965000000004</v>
+      </c>
+      <c r="T5" s="8">
         <v>2.1760000000000002</v>
       </c>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="2">
+      <c r="U5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="V5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="W5" s="17">
         <f>(S5-T5)/S5</f>
-        <v>-3.9074375856594248</v>
+        <v>0.60693616768001935</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
@@ -3315,75 +4793,45 @@
         <f>(K6-L6)/K6</f>
         <v>0.58161306613077823</v>
       </c>
-      <c r="Q6" s="1">
-        <v>256</v>
-      </c>
-      <c r="R6" s="1">
-        <v>300000</v>
-      </c>
-      <c r="S6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="T6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="U6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="V6" s="5"/>
-      <c r="W6" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="20"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="20"/>
+      <c r="W6" s="21"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="U7" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="V7" s="10"/>
-      <c r="W7" s="11"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="16"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="U8" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="V8" s="10"/>
-      <c r="W8" s="11"/>
+      <c r="U8" s="16"/>
+      <c r="V8" s="16"/>
     </row>
     <row r="30" spans="1:23" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="I30" s="8" t="s">
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="I30" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="Q30" s="9" t="s">
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="Q30" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="R30" s="9"/>
-      <c r="S30" s="9"/>
-      <c r="T30" s="9"/>
-      <c r="U30" s="9"/>
-      <c r="V30" s="14"/>
+      <c r="R30" s="13"/>
+      <c r="S30" s="13"/>
+      <c r="T30" s="13"/>
+      <c r="U30" s="13"/>
+      <c r="V30" s="11"/>
       <c r="W30" s="7"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.3">
@@ -3432,7 +4880,6 @@
       <c r="U31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="V31" s="11"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
@@ -3480,10 +4927,12 @@
         <v>8.1733399999999996E-4</v>
       </c>
       <c r="U32" s="2">
-        <f>(S32-T32)/S32</f>
-        <v>-53.488933333333328</v>
-      </c>
-      <c r="V32" s="12"/>
+        <f>(T32-S32)/T32</f>
+        <v>0.98164764955330375</v>
+      </c>
+      <c r="V32" s="14" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
@@ -3531,10 +4980,10 @@
         <v>0.17579239999999999</v>
       </c>
       <c r="U33" s="2">
-        <f t="shared" ref="U33:U34" si="0">(S33-T33)/S33</f>
-        <v>-6.3073284283160831</v>
-      </c>
-      <c r="V33" s="12"/>
+        <f t="shared" ref="U33:U34" si="0">(T33-S33)/T33</f>
+        <v>0.86315108047901956</v>
+      </c>
+      <c r="V33" s="9"/>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
@@ -3583,9 +5032,9 @@
       </c>
       <c r="U34" s="2">
         <f t="shared" si="0"/>
-        <v>-10.049835978997189</v>
-      </c>
-      <c r="V34" s="12"/>
+        <v>0.90950091911764708</v>
+      </c>
+      <c r="V34" s="9"/>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
@@ -3620,22 +5069,12 @@
         <f>(K35-L35)/K35</f>
         <v>0.78368503742665074</v>
       </c>
-      <c r="Q35" s="1">
-        <v>256</v>
-      </c>
-      <c r="R35" s="1">
-        <v>300000</v>
-      </c>
-      <c r="S35" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="T35" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="U35" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="V35" s="13"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="S35" s="4"/>
+      <c r="T35" s="4"/>
+      <c r="U35" s="6"/>
+      <c r="V35" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>